<commit_message>
update of nutritional recommendations
</commit_message>
<xml_diff>
--- a/DGE_recommendations.xlsx
+++ b/DGE_recommendations.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/321e4917f5e22f1c/Desktop/IT-Projekte/Multidimensional_Nutri-Score/Code/Multidimensional-Nutri-Score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03962255-4955-4F35-8BDF-772533F35B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="304" documentId="8_{03962255-4955-4F35-8BDF-772533F35B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFCB295A-9D2F-4767-8764-AADC5D232094}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Referenzwerte df" sheetId="1" r:id="rId1"/>
-    <sheet name="Fußnoten" sheetId="2" r:id="rId2"/>
-    <sheet name="recommendations" sheetId="3" r:id="rId3"/>
-    <sheet name="avg_recom" sheetId="6" r:id="rId4"/>
+    <sheet name="avg_vitamins" sheetId="7" r:id="rId1"/>
+    <sheet name="avg_recom" sheetId="6" r:id="rId2"/>
+    <sheet name="Referenzwerte df" sheetId="1" r:id="rId3"/>
+    <sheet name="Fußnoten" sheetId="2" r:id="rId4"/>
+    <sheet name="recommendations" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="218">
   <si>
     <t>Bevölkerungsgruppe</t>
   </si>
@@ -639,10 +640,79 @@
     <t>min</t>
   </si>
   <si>
-    <t>mittel</t>
-  </si>
-  <si>
     <t>avg</t>
+  </si>
+  <si>
+    <t>Energie (kcal/Tag)</t>
+  </si>
+  <si>
+    <t>Bezeichnung</t>
+  </si>
+  <si>
+    <t>Menge</t>
+  </si>
+  <si>
+    <t>Weiter Angabe</t>
+  </si>
+  <si>
+    <t>max (avg)</t>
+  </si>
+  <si>
+    <t>A (Retinoläquivalent)</t>
+  </si>
+  <si>
+    <t>A (Retinol)</t>
+  </si>
+  <si>
+    <t>A (Beta-Carotin)</t>
+  </si>
+  <si>
+    <t>B1 (Thiamin)</t>
+  </si>
+  <si>
+    <t>B2 (Riboflavin)</t>
+  </si>
+  <si>
+    <t>B3 (Niacin, Nicotinsäure)</t>
+  </si>
+  <si>
+    <t>B3 (Niacinäquivalent)</t>
+  </si>
+  <si>
+    <t>B5 (Pantothensäure)</t>
+  </si>
+  <si>
+    <t>B6 (Pyridoxin)</t>
+  </si>
+  <si>
+    <t>B7 (Biotin (Vitamin H))</t>
+  </si>
+  <si>
+    <t>B9 (gesamte Folsäure)</t>
+  </si>
+  <si>
+    <t>B12 (Cobalamin)</t>
+  </si>
+  <si>
+    <t>C (Ascorbinsäure)</t>
+  </si>
+  <si>
+    <t>D (Calciferole)</t>
+  </si>
+  <si>
+    <t>E (Tocopherole)</t>
+  </si>
+  <si>
+    <t>K ()</t>
+  </si>
+  <si>
+    <t>Quelle</t>
+  </si>
+  <si>
+    <t>naehrwertrechner.de</t>
+  </si>
+  <si>
+    <t>DGE</t>
   </si>
 </sst>
 </file>
@@ -697,6 +767,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1020,20 +1094,1286 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H92"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F32006-BDCD-4040-96C8-0A9582070BD1}">
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K1" t="s">
+        <v>208</v>
+      </c>
+      <c r="L1" t="s">
+        <v>209</v>
+      </c>
+      <c r="M1" t="s">
+        <v>210</v>
+      </c>
+      <c r="N1" t="s">
+        <v>211</v>
+      </c>
+      <c r="O1" t="s">
+        <v>212</v>
+      </c>
+      <c r="P1" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" t="s">
+        <v>61</v>
+      </c>
+      <c r="P2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3">
+        <v>900</v>
+      </c>
+      <c r="C3">
+        <v>2000</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>1100</v>
+      </c>
+      <c r="F3">
+        <v>1200</v>
+      </c>
+      <c r="G3">
+        <v>15000</v>
+      </c>
+      <c r="H3">
+        <v>17000</v>
+      </c>
+      <c r="I3">
+        <v>6000</v>
+      </c>
+      <c r="J3">
+        <v>16000</v>
+      </c>
+      <c r="K3">
+        <v>45</v>
+      </c>
+      <c r="L3">
+        <v>400</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>100000</v>
+      </c>
+      <c r="O3">
+        <v>20</v>
+      </c>
+      <c r="P3">
+        <v>14000</v>
+      </c>
+      <c r="Q3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F4" t="s">
+        <v>193</v>
+      </c>
+      <c r="G4" t="s">
+        <v>193</v>
+      </c>
+      <c r="I4" t="s">
+        <v>193</v>
+      </c>
+      <c r="N4" t="s">
+        <v>193</v>
+      </c>
+      <c r="O4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P4" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" t="s">
+        <v>81</v>
+      </c>
+      <c r="N6" t="s">
+        <v>90</v>
+      </c>
+      <c r="O6" t="s">
+        <v>63</v>
+      </c>
+      <c r="P6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E7" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" t="s">
+        <v>217</v>
+      </c>
+      <c r="G7" t="s">
+        <v>216</v>
+      </c>
+      <c r="H7" t="s">
+        <v>216</v>
+      </c>
+      <c r="I7" t="s">
+        <v>216</v>
+      </c>
+      <c r="J7" t="s">
+        <v>217</v>
+      </c>
+      <c r="K7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L7" t="s">
+        <v>217</v>
+      </c>
+      <c r="M7" t="s">
+        <v>217</v>
+      </c>
+      <c r="N7" t="s">
+        <v>217</v>
+      </c>
+      <c r="O7" t="s">
+        <v>217</v>
+      </c>
+      <c r="P7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265B2FAF-ABBA-4113-9E4F-E2409CE22460}">
+  <dimension ref="A1:AP6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.19921875" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="24.09765625" customWidth="1"/>
+    <col min="8" max="8" width="11.19921875" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="13" max="13" width="9.796875" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="22" max="22" width="9.09765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="str">
+        <f>IF(ISBLANK(recommendations!H1),"",recommendations!H1)</f>
+        <v>Protein</v>
+      </c>
+      <c r="E1" t="str">
+        <f>IF(ISBLANK(recommendations!I1),"",recommendations!I1)</f>
+        <v>Gesättigte Fettsäuren</v>
+      </c>
+      <c r="F1" t="str">
+        <f>IF(ISBLANK(recommendations!J1),"",recommendations!J1)</f>
+        <v>Einfach ungesättigte Fettsäuren</v>
+      </c>
+      <c r="G1" t="str">
+        <f>IF(ISBLANK(recommendations!K1),"",recommendations!K1)</f>
+        <v>Mehrfach ungesättigte Fettsäuren</v>
+      </c>
+      <c r="H1" t="str">
+        <f>IF(ISBLANK(recommendations!L1),"",recommendations!L1)</f>
+        <v>Linolsäure</v>
+      </c>
+      <c r="I1" t="str">
+        <f>IF(ISBLANK(recommendations!M1),"",recommendations!M1)</f>
+        <v>α-Linolensäure</v>
+      </c>
+      <c r="J1" t="str">
+        <f>IF(ISBLANK(recommendations!N1),"",recommendations!N1)</f>
+        <v>EPA_DHA</v>
+      </c>
+      <c r="K1" t="str">
+        <f>IF(ISBLANK(recommendations!O1),"",recommendations!O1)</f>
+        <v>Kohlenhydrate</v>
+      </c>
+      <c r="L1" t="str">
+        <f>IF(ISBLANK(recommendations!P1),"",recommendations!P1)</f>
+        <v>Ballaststoffe</v>
+      </c>
+      <c r="M1" t="str">
+        <f>IF(ISBLANK(recommendations!Q1),"",recommendations!Q1)</f>
+        <v>Alkohol</v>
+      </c>
+      <c r="N1" t="str">
+        <f>IF(ISBLANK(recommendations!R1),"",recommendations!R1)</f>
+        <v>Vitamin A</v>
+      </c>
+      <c r="O1" t="str">
+        <f>IF(ISBLANK(recommendations!S1),"",recommendations!S1)</f>
+        <v>Vitamin D</v>
+      </c>
+      <c r="P1" t="str">
+        <f>IF(ISBLANK(recommendations!T1),"",recommendations!T1)</f>
+        <v>Vitamin E</v>
+      </c>
+      <c r="Q1" t="str">
+        <f>IF(ISBLANK(recommendations!U1),"",recommendations!U1)</f>
+        <v>Vitamin K</v>
+      </c>
+      <c r="R1" t="str">
+        <f>IF(ISBLANK(recommendations!V1),"",recommendations!V1)</f>
+        <v>Thiamin</v>
+      </c>
+      <c r="S1" t="str">
+        <f>IF(ISBLANK(recommendations!W1),"",recommendations!W1)</f>
+        <v>Riboflavin</v>
+      </c>
+      <c r="T1" t="str">
+        <f>IF(ISBLANK(recommendations!X1),"",recommendations!X1)</f>
+        <v>Niacin</v>
+      </c>
+      <c r="U1" t="str">
+        <f>IF(ISBLANK(recommendations!Y1),"",recommendations!Y1)</f>
+        <v>Vitamin B6</v>
+      </c>
+      <c r="V1" t="str">
+        <f>IF(ISBLANK(recommendations!Z1),"",recommendations!Z1)</f>
+        <v>Folat</v>
+      </c>
+      <c r="W1" t="str">
+        <f>IF(ISBLANK(recommendations!AA1),"",recommendations!AA1)</f>
+        <v>Pantothensäure</v>
+      </c>
+      <c r="X1" t="str">
+        <f>IF(ISBLANK(recommendations!AB1),"",recommendations!AB1)</f>
+        <v>Biotin</v>
+      </c>
+      <c r="Y1" t="str">
+        <f>IF(ISBLANK(recommendations!AC1),"",recommendations!AC1)</f>
+        <v>Vitamin B12 (Cobalamine)</v>
+      </c>
+      <c r="Z1" t="str">
+        <f>IF(ISBLANK(recommendations!AD1),"",recommendations!AD1)</f>
+        <v>Vitamin C</v>
+      </c>
+      <c r="AA1" t="str">
+        <f>IF(ISBLANK(recommendations!AE1),"",recommendations!AE1)</f>
+        <v>Natrium</v>
+      </c>
+      <c r="AB1" t="str">
+        <f>IF(ISBLANK(recommendations!AF1),"",recommendations!AF1)</f>
+        <v>Chlorid</v>
+      </c>
+      <c r="AC1" t="str">
+        <f>IF(ISBLANK(recommendations!AG1),"",recommendations!AG1)</f>
+        <v>Kalium</v>
+      </c>
+      <c r="AD1" t="str">
+        <f>IF(ISBLANK(recommendations!AH1),"",recommendations!AH1)</f>
+        <v>Calcium</v>
+      </c>
+      <c r="AE1" t="str">
+        <f>IF(ISBLANK(recommendations!AI1),"",recommendations!AI1)</f>
+        <v>Phosphor</v>
+      </c>
+      <c r="AF1" t="str">
+        <f>IF(ISBLANK(recommendations!AJ1),"",recommendations!AJ1)</f>
+        <v>Magnesium</v>
+      </c>
+      <c r="AG1" t="str">
+        <f>IF(ISBLANK(recommendations!AK1),"",recommendations!AK1)</f>
+        <v>Eisen</v>
+      </c>
+      <c r="AH1" t="str">
+        <f>IF(ISBLANK(recommendations!AL1),"",recommendations!AL1)</f>
+        <v>Jod</v>
+      </c>
+      <c r="AI1" t="str">
+        <f>IF(ISBLANK(recommendations!AM1),"",recommendations!AM1)</f>
+        <v>Fluorid</v>
+      </c>
+      <c r="AJ1" t="str">
+        <f>IF(ISBLANK(recommendations!AN1),"",recommendations!AN1)</f>
+        <v>Zink</v>
+      </c>
+      <c r="AK1" t="str">
+        <f>IF(ISBLANK(recommendations!AQ1),"",recommendations!AQ1)</f>
+        <v>Selen</v>
+      </c>
+      <c r="AL1" t="str">
+        <f>IF(ISBLANK(recommendations!AR1),"",recommendations!AR1)</f>
+        <v>Kupfer</v>
+      </c>
+      <c r="AM1" t="str">
+        <f>IF(ISBLANK(recommendations!AS1),"",recommendations!AS1)</f>
+        <v>Mangan</v>
+      </c>
+      <c r="AN1" t="str">
+        <f>IF(ISBLANK(recommendations!AT1),"",recommendations!AT1)</f>
+        <v>Chrom</v>
+      </c>
+      <c r="AO1" t="str">
+        <f>IF(ISBLANK(recommendations!AU1),"",recommendations!AU1)</f>
+        <v>Molybdän</v>
+      </c>
+      <c r="AP1" t="str">
+        <f>IF(ISBLANK(recommendations!AV1),"",recommendations!AV1)</f>
+        <v>Wasser</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="str">
+        <f>IF(ISBLANK(recommendations!F2),"",recommendations!F2)</f>
+        <v>kcal/Tag</v>
+      </c>
+      <c r="C2" t="str">
+        <f>IF(ISBLANK(recommendations!G2),"",recommendations!G2)</f>
+        <v>% der Energie</v>
+      </c>
+      <c r="D2" t="str">
+        <f>IF(ISBLANK(recommendations!H2),"",recommendations!H2)</f>
+        <v>g/kg KG/Tag</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(ISBLANK(recommendations!I2),"",recommendations!I2)</f>
+        <v>% der Energie</v>
+      </c>
+      <c r="F2" t="str">
+        <f>IF(ISBLANK(recommendations!J2),"",recommendations!J2)</f>
+        <v>% der Energie</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IF(ISBLANK(recommendations!K2),"",recommendations!K2)</f>
+        <v>% der Energie</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(ISBLANK(recommendations!L2),"",recommendations!L2)</f>
+        <v>% der Energie</v>
+      </c>
+      <c r="I2" t="str">
+        <f>IF(ISBLANK(recommendations!M2),"",recommendations!M2)</f>
+        <v>% der Energie</v>
+      </c>
+      <c r="J2" t="str">
+        <f>IF(ISBLANK(recommendations!N2),"",recommendations!N2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="K2" t="str">
+        <f>IF(ISBLANK(recommendations!O2),"",recommendations!O2)</f>
+        <v>% der Energie</v>
+      </c>
+      <c r="L2" t="str">
+        <f>IF(ISBLANK(recommendations!P2),"",recommendations!P2)</f>
+        <v>g/Tag</v>
+      </c>
+      <c r="M2" t="str">
+        <f>IF(ISBLANK(recommendations!Q2),"",recommendations!Q2)</f>
+        <v>g/Tag</v>
+      </c>
+      <c r="N2" t="str">
+        <f>IF(ISBLANK(recommendations!R2),"",recommendations!R2)</f>
+        <v>µg-RAE/Tag</v>
+      </c>
+      <c r="O2" t="str">
+        <f>IF(ISBLANK(recommendations!S2),"",recommendations!S2)</f>
+        <v>µg/Tag</v>
+      </c>
+      <c r="P2" t="str">
+        <f>IF(ISBLANK(recommendations!T2),"",recommendations!T2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>IF(ISBLANK(recommendations!U2),"",recommendations!U2)</f>
+        <v>µg/Tag</v>
+      </c>
+      <c r="R2" t="str">
+        <f>IF(ISBLANK(recommendations!V2),"",recommendations!V2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="S2" t="str">
+        <f>IF(ISBLANK(recommendations!W2),"",recommendations!W2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="T2" t="str">
+        <f>IF(ISBLANK(recommendations!X2),"",recommendations!X2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="U2" t="str">
+        <f>IF(ISBLANK(recommendations!Y2),"",recommendations!Y2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="V2" t="str">
+        <f>IF(ISBLANK(recommendations!Z2),"",recommendations!Z2)</f>
+        <v>µg/Tag</v>
+      </c>
+      <c r="W2" t="str">
+        <f>IF(ISBLANK(recommendations!AA2),"",recommendations!AA2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="X2" t="str">
+        <f>IF(ISBLANK(recommendations!AB2),"",recommendations!AB2)</f>
+        <v>µg/Tag</v>
+      </c>
+      <c r="Y2" t="str">
+        <f>IF(ISBLANK(recommendations!AC2),"",recommendations!AC2)</f>
+        <v>µg/Tag</v>
+      </c>
+      <c r="Z2" t="str">
+        <f>IF(ISBLANK(recommendations!AD2),"",recommendations!AD2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="AA2" t="str">
+        <f>IF(ISBLANK(recommendations!AE2),"",recommendations!AE2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="AB2" t="str">
+        <f>IF(ISBLANK(recommendations!AF2),"",recommendations!AF2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="AC2" t="str">
+        <f>IF(ISBLANK(recommendations!AG2),"",recommendations!AG2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="AD2" t="str">
+        <f>IF(ISBLANK(recommendations!AH2),"",recommendations!AH2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="AE2" t="str">
+        <f>IF(ISBLANK(recommendations!AI2),"",recommendations!AI2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="AF2" t="str">
+        <f>IF(ISBLANK(recommendations!AJ2),"",recommendations!AJ2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="AG2" t="str">
+        <f>IF(ISBLANK(recommendations!AK2),"",recommendations!AK2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="AH2" t="str">
+        <f>IF(ISBLANK(recommendations!AL2),"",recommendations!AL2)</f>
+        <v>µg/Tag</v>
+      </c>
+      <c r="AI2" t="str">
+        <f>IF(ISBLANK(recommendations!AM2),"",recommendations!AM2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="AJ2" t="str">
+        <f>IF(ISBLANK(recommendations!AN2),"",recommendations!AN2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="AK2" t="str">
+        <f>IF(ISBLANK(recommendations!AQ2),"",recommendations!AQ2)</f>
+        <v>µg/Tag</v>
+      </c>
+      <c r="AL2" t="str">
+        <f>IF(ISBLANK(recommendations!AR2),"",recommendations!AR2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="AM2" t="str">
+        <f>IF(ISBLANK(recommendations!AS2),"",recommendations!AS2)</f>
+        <v>mg/Tag</v>
+      </c>
+      <c r="AN2" t="str">
+        <f>IF(ISBLANK(recommendations!AT2),"",recommendations!AT2)</f>
+        <v>µg/Tag</v>
+      </c>
+      <c r="AO2" t="str">
+        <f>IF(ISBLANK(recommendations!AU2),"",recommendations!AU2)</f>
+        <v>µg/Tag</v>
+      </c>
+      <c r="AP2" t="str">
+        <f>IF(ISBLANK(recommendations!AV2),"",recommendations!AV2)</f>
+        <v>ml/Tag</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3">
+        <f>(2100+2667)/2</f>
+        <v>2383.5</v>
+      </c>
+      <c r="C3">
+        <f>0.3*B3/9</f>
+        <v>79.449999999999989</v>
+      </c>
+      <c r="D3">
+        <f>72.5*1</f>
+        <v>72.5</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <f>$B$3*0.1/9</f>
+        <v>26.483333333333334</v>
+      </c>
+      <c r="G3">
+        <f>$B$3*0.085/9</f>
+        <v>22.510833333333338</v>
+      </c>
+      <c r="H3">
+        <f>$B$3*0.025/9</f>
+        <v>6.6208333333333336</v>
+      </c>
+      <c r="I3">
+        <f>$B$3*0.05/9</f>
+        <v>13.241666666666667</v>
+      </c>
+      <c r="J3">
+        <v>250</v>
+      </c>
+      <c r="K3">
+        <f>$B$3*0.05/9</f>
+        <v>13.241666666666667</v>
+      </c>
+      <c r="L3">
+        <v>30</v>
+      </c>
+      <c r="M3">
+        <v>15</v>
+      </c>
+      <c r="N3">
+        <f>(700+850)/2</f>
+        <v>775</v>
+      </c>
+      <c r="O3">
+        <v>20</v>
+      </c>
+      <c r="P3">
+        <v>13</v>
+      </c>
+      <c r="Q3">
+        <v>65</v>
+      </c>
+      <c r="R3">
+        <f>(1+1.2)/2</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S3">
+        <f>(1.1+1.4)/2</f>
+        <v>1.25</v>
+      </c>
+      <c r="T3">
+        <f>(12+15)/2</f>
+        <v>13.5</v>
+      </c>
+      <c r="U3">
+        <f>(1.4+1.6)/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="V3">
+        <v>300</v>
+      </c>
+      <c r="W3">
+        <v>5</v>
+      </c>
+      <c r="X3">
+        <v>40</v>
+      </c>
+      <c r="Y3">
+        <v>4</v>
+      </c>
+      <c r="Z3">
+        <f>100</f>
+        <v>100</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF3">
+        <v>325</v>
+      </c>
+      <c r="AG3">
+        <f>(15+10)/2</f>
+        <v>12.5</v>
+      </c>
+      <c r="AH3">
+        <v>200</v>
+      </c>
+      <c r="AI3">
+        <f>(3.1+3.8)/2</f>
+        <v>3.45</v>
+      </c>
+      <c r="AJ3">
+        <f>(8.3+13.7)/2</f>
+        <v>11</v>
+      </c>
+      <c r="AK3">
+        <v>65</v>
+      </c>
+      <c r="AL3">
+        <v>1.25</v>
+      </c>
+      <c r="AM3">
+        <v>3.5</v>
+      </c>
+      <c r="AN3">
+        <v>65</v>
+      </c>
+      <c r="AO3">
+        <v>75</v>
+      </c>
+      <c r="AP3">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="str">
+        <f>IF(ISBLANK(recommendations!G3),"",recommendations!G3)</f>
+        <v/>
+      </c>
+      <c r="D4" t="str">
+        <f>IF(ISBLANK(recommendations!H3),"",recommendations!H3)</f>
+        <v/>
+      </c>
+      <c r="E4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" t="s">
+        <v>192</v>
+      </c>
+      <c r="H4" t="str">
+        <f>IF(ISBLANK(recommendations!L3),"",recommendations!L3)</f>
+        <v/>
+      </c>
+      <c r="I4" t="str">
+        <f>IF(ISBLANK(recommendations!M3),"",recommendations!M3)</f>
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <f>IF(ISBLANK(recommendations!N3),"",recommendations!N3)</f>
+        <v/>
+      </c>
+      <c r="K4" t="s">
+        <v>192</v>
+      </c>
+      <c r="L4" t="s">
+        <v>192</v>
+      </c>
+      <c r="M4" t="s">
+        <v>198</v>
+      </c>
+      <c r="N4" t="s">
+        <v>193</v>
+      </c>
+      <c r="O4" t="str">
+        <f>IF(ISBLANK(recommendations!S3),"",recommendations!S3)</f>
+        <v>bei fehlender endogener Synthese</v>
+      </c>
+      <c r="P4" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>193</v>
+      </c>
+      <c r="R4" t="s">
+        <v>193</v>
+      </c>
+      <c r="S4" t="s">
+        <v>193</v>
+      </c>
+      <c r="T4" t="s">
+        <v>193</v>
+      </c>
+      <c r="U4" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" t="str">
+        <f>IF(ISBLANK(recommendations!D4),"",recommendations!D4)</f>
+        <v>Richtwert</v>
+      </c>
+      <c r="C5" t="str">
+        <f>IF(ISBLANK(recommendations!G4),"",recommendations!G4)</f>
+        <v>Richtwert</v>
+      </c>
+      <c r="D5" t="str">
+        <f>IF(ISBLANK(recommendations!H4),"",recommendations!H4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="F5" t="str">
+        <f>IF(ISBLANK(recommendations!J4),"",recommendations!J4)</f>
+        <v>-</v>
+      </c>
+      <c r="G5" t="str">
+        <f>IF(ISBLANK(recommendations!K4),"",recommendations!K4)</f>
+        <v>-</v>
+      </c>
+      <c r="H5" t="str">
+        <f>IF(ISBLANK(recommendations!L4),"",recommendations!L4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="I5" t="str">
+        <f>IF(ISBLANK(recommendations!M4),"",recommendations!M4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="J5" t="str">
+        <f>IF(ISBLANK(recommendations!N4),"",recommendations!N4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="K5" t="str">
+        <f>IF(ISBLANK(recommendations!O4),"",recommendations!O4)</f>
+        <v>Richtwert</v>
+      </c>
+      <c r="L5" t="str">
+        <f>IF(ISBLANK(recommendations!P4),"",recommendations!P4)</f>
+        <v>Richtwert</v>
+      </c>
+      <c r="M5" t="str">
+        <f>IF(ISBLANK(recommendations!Q4),"",recommendations!Q4)</f>
+        <v>Richtwert</v>
+      </c>
+      <c r="N5" t="str">
+        <f>IF(ISBLANK(recommendations!R4),"",recommendations!R4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="O5" t="str">
+        <f>IF(ISBLANK(recommendations!S4),"",recommendations!S4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="P5" t="str">
+        <f>IF(ISBLANK(recommendations!T4),"",recommendations!T4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="Q5" t="str">
+        <f>IF(ISBLANK(recommendations!U4),"",recommendations!U4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="R5" t="str">
+        <f>IF(ISBLANK(recommendations!V4),"",recommendations!V4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="S5" t="str">
+        <f>IF(ISBLANK(recommendations!W4),"",recommendations!W4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="T5" t="str">
+        <f>IF(ISBLANK(recommendations!X4),"",recommendations!X4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="U5" t="str">
+        <f>IF(ISBLANK(recommendations!Y4),"",recommendations!Y4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="V5" t="str">
+        <f>IF(ISBLANK(recommendations!Z4),"",recommendations!Z4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="W5" t="str">
+        <f>IF(ISBLANK(recommendations!AA4),"",recommendations!AA4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="X5" t="str">
+        <f>IF(ISBLANK(recommendations!AB4),"",recommendations!AB4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="Y5" t="str">
+        <f>IF(ISBLANK(recommendations!AC4),"",recommendations!AC4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="Z5" t="str">
+        <f>IF(ISBLANK(recommendations!AD4),"",recommendations!AD4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="AA5" t="str">
+        <f>IF(ISBLANK(recommendations!AE4),"",recommendations!AE4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="AB5" t="str">
+        <f>IF(ISBLANK(recommendations!AF4),"",recommendations!AF4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="AC5" t="str">
+        <f>IF(ISBLANK(recommendations!AG4),"",recommendations!AG4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="AD5" t="str">
+        <f>IF(ISBLANK(recommendations!AH4),"",recommendations!AH4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="AE5" t="str">
+        <f>IF(ISBLANK(recommendations!AI4),"",recommendations!AI4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="AF5" t="str">
+        <f>IF(ISBLANK(recommendations!AJ4),"",recommendations!AJ4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="AG5" t="str">
+        <f>IF(ISBLANK(recommendations!AK4),"",recommendations!AK4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="AH5" t="str">
+        <f>IF(ISBLANK(recommendations!AL4),"",recommendations!AL4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="AI5" t="str">
+        <f>IF(ISBLANK(recommendations!AM4),"",recommendations!AM4)</f>
+        <v>Richtwert</v>
+      </c>
+      <c r="AJ5" t="str">
+        <f>IF(ISBLANK(recommendations!AN4),"",recommendations!AN4)</f>
+        <v>Empfohlene Zufuhr</v>
+      </c>
+      <c r="AK5" t="str">
+        <f>IF(ISBLANK(recommendations!AQ4),"",recommendations!AQ4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="AL5" t="str">
+        <f>IF(ISBLANK(recommendations!AR4),"",recommendations!AR4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="AM5" t="str">
+        <f>IF(ISBLANK(recommendations!AS4),"",recommendations!AS4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="AN5" t="str">
+        <f>IF(ISBLANK(recommendations!AT4),"",recommendations!AT4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="AO5" t="str">
+        <f>IF(ISBLANK(recommendations!AU4),"",recommendations!AU4)</f>
+        <v>Schätzwert</v>
+      </c>
+      <c r="AP5" t="str">
+        <f>IF(ISBLANK(recommendations!AV4),"",recommendations!AV4)</f>
+        <v>Richtwert</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="str">
+        <f>IF(ISBLANK(recommendations!D5),"",recommendations!D5)</f>
+        <v/>
+      </c>
+      <c r="C6" t="str">
+        <f>IF(ISBLANK(recommendations!G5),"",recommendations!G5)</f>
+        <v>ag,aj,c,af</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(ISBLANK(recommendations!H5),"",recommendations!H5)</f>
+        <v>a</v>
+      </c>
+      <c r="E6" t="str">
+        <f>IF(ISBLANK(recommendations!I5),"",recommendations!I5)</f>
+        <v/>
+      </c>
+      <c r="F6" t="str">
+        <f>IF(ISBLANK(recommendations!J5),"",recommendations!J5)</f>
+        <v/>
+      </c>
+      <c r="G6" t="str">
+        <f>IF(ISBLANK(recommendations!K5),"",recommendations!K5)</f>
+        <v/>
+      </c>
+      <c r="H6" t="str">
+        <f>IF(ISBLANK(recommendations!L5),"",recommendations!L5)</f>
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <f>IF(ISBLANK(recommendations!M5),"",recommendations!M5)</f>
+        <v/>
+      </c>
+      <c r="J6" t="str">
+        <f>IF(ISBLANK(recommendations!N5),"",recommendations!N5)</f>
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <f>IF(ISBLANK(recommendations!O5),"",recommendations!O5)</f>
+        <v>ai,aj</v>
+      </c>
+      <c r="L6" t="str">
+        <f>IF(ISBLANK(recommendations!P5),"",recommendations!P5)</f>
+        <v>ap</v>
+      </c>
+      <c r="M6" t="str">
+        <f>IF(ISBLANK(recommendations!Q5),"",recommendations!Q5)</f>
+        <v>ak</v>
+      </c>
+      <c r="N6" t="str">
+        <f>IF(ISBLANK(recommendations!R5),"",recommendations!R5)</f>
+        <v>d</v>
+      </c>
+      <c r="O6" t="str">
+        <f>IF(ISBLANK(recommendations!S5),"",recommendations!S5)</f>
+        <v>e,al</v>
+      </c>
+      <c r="P6" t="str">
+        <f>IF(ISBLANK(recommendations!T5),"",recommendations!T5)</f>
+        <v>g</v>
+      </c>
+      <c r="Q6" t="str">
+        <f>IF(ISBLANK(recommendations!U5),"",recommendations!U5)</f>
+        <v/>
+      </c>
+      <c r="R6" t="str">
+        <f>IF(ISBLANK(recommendations!V5),"",recommendations!V5)</f>
+        <v>j</v>
+      </c>
+      <c r="S6" t="str">
+        <f>IF(ISBLANK(recommendations!W5),"",recommendations!W5)</f>
+        <v>j</v>
+      </c>
+      <c r="T6" t="str">
+        <f>IF(ISBLANK(recommendations!X5),"",recommendations!X5)</f>
+        <v>i,j</v>
+      </c>
+      <c r="U6" t="str">
+        <f>IF(ISBLANK(recommendations!Y5),"",recommendations!Y5)</f>
+        <v/>
+      </c>
+      <c r="V6" t="str">
+        <f>IF(ISBLANK(recommendations!Z5),"",recommendations!Z5)</f>
+        <v>m,n</v>
+      </c>
+      <c r="W6" t="str">
+        <f>IF(ISBLANK(recommendations!AA5),"",recommendations!AA5)</f>
+        <v/>
+      </c>
+      <c r="X6" t="str">
+        <f>IF(ISBLANK(recommendations!AB5),"",recommendations!AB5)</f>
+        <v/>
+      </c>
+      <c r="Y6" t="str">
+        <f>IF(ISBLANK(recommendations!AC5),"",recommendations!AC5)</f>
+        <v/>
+      </c>
+      <c r="Z6" t="str">
+        <f>IF(ISBLANK(recommendations!AD5),"",recommendations!AD5)</f>
+        <v>p</v>
+      </c>
+      <c r="AA6" t="str">
+        <f>IF(ISBLANK(recommendations!AE5),"",recommendations!AE5)</f>
+        <v/>
+      </c>
+      <c r="AB6" t="str">
+        <f>IF(ISBLANK(recommendations!AF5),"",recommendations!AF5)</f>
+        <v/>
+      </c>
+      <c r="AC6" t="str">
+        <f>IF(ISBLANK(recommendations!AG5),"",recommendations!AG5)</f>
+        <v/>
+      </c>
+      <c r="AD6" t="str">
+        <f>IF(ISBLANK(recommendations!AH5),"",recommendations!AH5)</f>
+        <v/>
+      </c>
+      <c r="AE6" t="str">
+        <f>IF(ISBLANK(recommendations!AI5),"",recommendations!AI5)</f>
+        <v/>
+      </c>
+      <c r="AF6" t="str">
+        <f>IF(ISBLANK(recommendations!AJ5),"",recommendations!AJ5)</f>
+        <v/>
+      </c>
+      <c r="AG6" t="str">
+        <f>IF(ISBLANK(recommendations!AK5),"",recommendations!AK5)</f>
+        <v>v</v>
+      </c>
+      <c r="AH6" t="str">
+        <f>IF(ISBLANK(recommendations!AL5),"",recommendations!AL5)</f>
+        <v/>
+      </c>
+      <c r="AI6" t="str">
+        <f>IF(ISBLANK(recommendations!AM5),"",recommendations!AM5)</f>
+        <v>am,an</v>
+      </c>
+      <c r="AJ6" t="str">
+        <f>IF(ISBLANK(recommendations!AN5),"",recommendations!AN5)</f>
+        <v>x,y1</v>
+      </c>
+      <c r="AK6" t="str">
+        <f>IF(ISBLANK(recommendations!AQ5),"",recommendations!AQ5)</f>
+        <v/>
+      </c>
+      <c r="AL6" t="str">
+        <f>IF(ISBLANK(recommendations!AR5),"",recommendations!AR5)</f>
+        <v/>
+      </c>
+      <c r="AM6" t="str">
+        <f>IF(ISBLANK(recommendations!AS5),"",recommendations!AS5)</f>
+        <v/>
+      </c>
+      <c r="AN6" t="str">
+        <f>IF(ISBLANK(recommendations!AT5),"",recommendations!AT5)</f>
+        <v/>
+      </c>
+      <c r="AO6" t="str">
+        <f>IF(ISBLANK(recommendations!AU5),"",recommendations!AU5)</f>
+        <v/>
+      </c>
+      <c r="AP6" t="str">
+        <f>IF(ISBLANK(recommendations!AV5),"",recommendations!AV5)</f>
+        <v>s</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H91"/>
+  <sheetViews>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.59765625" customWidth="1"/>
     <col min="3" max="3" width="22.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1059,7 +2399,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1085,7 +2425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1111,7 +2451,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1137,7 +2477,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1163,7 +2503,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1189,7 +2529,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1215,7 +2555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1241,7 +2581,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1267,7 +2607,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +2633,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1319,7 +2659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1345,7 +2685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1371,7 +2711,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1397,7 +2737,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1423,7 +2763,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1449,7 +2789,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1475,7 +2815,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1501,7 +2841,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1527,7 +2867,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1553,7 +2893,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1579,7 +2919,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1605,7 +2945,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1631,7 +2971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1657,7 +2997,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1683,7 +3023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1709,7 +3049,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1735,7 +3075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1761,7 +3101,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1787,7 +3127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1813,7 +3153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1839,7 +3179,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1865,7 +3205,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1891,7 +3231,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1917,7 +3257,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1943,7 +3283,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1969,7 +3309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1995,7 +3335,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -2021,7 +3361,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -2047,7 +3387,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -2073,7 +3413,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -2099,7 +3439,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -2125,7 +3465,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -2151,7 +3491,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -2177,7 +3517,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2203,7 +3543,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -2229,7 +3569,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>174</v>
       </c>
@@ -2255,7 +3595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>174</v>
       </c>
@@ -2281,7 +3621,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>174</v>
       </c>
@@ -2307,7 +3647,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>174</v>
       </c>
@@ -2333,7 +3673,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>174</v>
       </c>
@@ -2359,7 +3699,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>174</v>
       </c>
@@ -2385,7 +3725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>174</v>
       </c>
@@ -2411,7 +3751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>174</v>
       </c>
@@ -2437,7 +3777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>174</v>
       </c>
@@ -2463,7 +3803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>174</v>
       </c>
@@ -2489,7 +3829,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>174</v>
       </c>
@@ -2515,7 +3855,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>174</v>
       </c>
@@ -2541,7 +3881,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>174</v>
       </c>
@@ -2567,7 +3907,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>174</v>
       </c>
@@ -2593,7 +3933,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>174</v>
       </c>
@@ -2619,7 +3959,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>174</v>
       </c>
@@ -2645,7 +3985,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>174</v>
       </c>
@@ -2671,7 +4011,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>174</v>
       </c>
@@ -2697,7 +4037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>174</v>
       </c>
@@ -2723,7 +4063,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>174</v>
       </c>
@@ -2749,7 +4089,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>174</v>
       </c>
@@ -2775,7 +4115,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>174</v>
       </c>
@@ -2801,7 +4141,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>174</v>
       </c>
@@ -2827,7 +4167,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>174</v>
       </c>
@@ -2853,7 +4193,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>174</v>
       </c>
@@ -2879,7 +4219,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>174</v>
       </c>
@@ -2905,7 +4245,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>174</v>
       </c>
@@ -2931,7 +4271,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>174</v>
       </c>
@@ -2957,7 +4297,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>174</v>
       </c>
@@ -2983,7 +4323,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>174</v>
       </c>
@@ -3009,7 +4349,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>174</v>
       </c>
@@ -3035,7 +4375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>174</v>
       </c>
@@ -3061,7 +4401,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>174</v>
       </c>
@@ -3087,7 +4427,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>174</v>
       </c>
@@ -3113,7 +4453,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>174</v>
       </c>
@@ -3139,7 +4479,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>174</v>
       </c>
@@ -3165,7 +4505,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>174</v>
       </c>
@@ -3191,7 +4531,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>174</v>
       </c>
@@ -3217,7 +4557,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>174</v>
       </c>
@@ -3243,7 +4583,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>174</v>
       </c>
@@ -3269,7 +4609,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>174</v>
       </c>
@@ -3295,7 +4635,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>174</v>
       </c>
@@ -3321,7 +4661,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>174</v>
       </c>
@@ -3347,7 +4687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>174</v>
       </c>
@@ -3373,7 +4713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>174</v>
       </c>
@@ -3399,7 +4739,6 @@
         <v>130</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="15.6" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3408,7 +4747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
@@ -3416,9 +4755,9 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>131</v>
       </c>
@@ -3426,7 +4765,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -3434,7 +4773,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>134</v>
       </c>
@@ -3442,7 +4781,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -3450,7 +4789,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -3458,7 +4797,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -3466,7 +4805,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -3474,7 +4813,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -3482,7 +4821,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -3490,7 +4829,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>145</v>
       </c>
@@ -3498,7 +4837,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -3506,7 +4845,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>130</v>
       </c>
@@ -3514,7 +4853,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -3522,7 +4861,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>150</v>
       </c>
@@ -3530,7 +4869,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>152</v>
       </c>
@@ -3538,7 +4877,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>154</v>
       </c>
@@ -3546,7 +4885,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>156</v>
       </c>
@@ -3554,7 +4893,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>158</v>
       </c>
@@ -3562,7 +4901,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>160</v>
       </c>
@@ -3570,7 +4909,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>162</v>
       </c>
@@ -3578,7 +4917,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>164</v>
       </c>
@@ -3586,7 +4925,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -3594,7 +4933,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>167</v>
       </c>
@@ -3602,7 +4941,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>169</v>
       </c>
@@ -3610,7 +4949,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>171</v>
       </c>
@@ -3618,7 +4957,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -3634,18 +4973,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F5A0FC-0C73-492D-8E0C-7F7EF8032F1F}">
   <dimension ref="A1:AV10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="AA27" sqref="AA27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="28.296875" customWidth="1"/>
+    <col min="10" max="10" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.3">
@@ -4969,1231 +6309,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265B2FAF-ABBA-4113-9E4F-E2409CE22460}">
-  <dimension ref="A1:AR7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="7" max="7" width="19.19921875" customWidth="1"/>
-    <col min="9" max="9" width="24.09765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A1" t="str">
-        <f>IF(ISBLANK(recommendations!A1),"",recommendations!A1)</f>
-        <v>Wert</v>
-      </c>
-      <c r="B1" t="str">
-        <f>IF(ISBLANK(recommendations!B1),"",recommendations!B1)</f>
-        <v>Bevölkerungsgruppe</v>
-      </c>
-      <c r="C1" t="str">
-        <f>IF(ISBLANK(recommendations!C1),"",recommendations!C1)</f>
-        <v>Geschlecht</v>
-      </c>
-      <c r="D1" t="str">
-        <f>IF(ISBLANK(recommendations!D1),"",recommendations!D1)</f>
-        <v>Energie</v>
-      </c>
-      <c r="E1" t="str">
-        <f>IF(ISBLANK(recommendations!G1),"",recommendations!G1)</f>
-        <v>Gesamtfett</v>
-      </c>
-      <c r="F1" t="str">
-        <f>IF(ISBLANK(recommendations!H1),"",recommendations!H1)</f>
-        <v>Protein</v>
-      </c>
-      <c r="G1" t="str">
-        <f>IF(ISBLANK(recommendations!I1),"",recommendations!I1)</f>
-        <v>Gesättigte Fettsäuren</v>
-      </c>
-      <c r="H1" t="str">
-        <f>IF(ISBLANK(recommendations!J1),"",recommendations!J1)</f>
-        <v>Einfach ungesättigte Fettsäuren</v>
-      </c>
-      <c r="I1" t="str">
-        <f>IF(ISBLANK(recommendations!K1),"",recommendations!K1)</f>
-        <v>Mehrfach ungesättigte Fettsäuren</v>
-      </c>
-      <c r="J1" t="str">
-        <f>IF(ISBLANK(recommendations!L1),"",recommendations!L1)</f>
-        <v>Linolsäure</v>
-      </c>
-      <c r="K1" t="str">
-        <f>IF(ISBLANK(recommendations!M1),"",recommendations!M1)</f>
-        <v>α-Linolensäure</v>
-      </c>
-      <c r="L1" t="str">
-        <f>IF(ISBLANK(recommendations!N1),"",recommendations!N1)</f>
-        <v>EPA_DHA</v>
-      </c>
-      <c r="M1" t="str">
-        <f>IF(ISBLANK(recommendations!O1),"",recommendations!O1)</f>
-        <v>Kohlenhydrate</v>
-      </c>
-      <c r="N1" t="str">
-        <f>IF(ISBLANK(recommendations!P1),"",recommendations!P1)</f>
-        <v>Ballaststoffe</v>
-      </c>
-      <c r="O1" t="str">
-        <f>IF(ISBLANK(recommendations!Q1),"",recommendations!Q1)</f>
-        <v>Alkohol</v>
-      </c>
-      <c r="P1" t="str">
-        <f>IF(ISBLANK(recommendations!R1),"",recommendations!R1)</f>
-        <v>Vitamin A</v>
-      </c>
-      <c r="Q1" t="str">
-        <f>IF(ISBLANK(recommendations!S1),"",recommendations!S1)</f>
-        <v>Vitamin D</v>
-      </c>
-      <c r="R1" t="str">
-        <f>IF(ISBLANK(recommendations!T1),"",recommendations!T1)</f>
-        <v>Vitamin E</v>
-      </c>
-      <c r="S1" t="str">
-        <f>IF(ISBLANK(recommendations!U1),"",recommendations!U1)</f>
-        <v>Vitamin K</v>
-      </c>
-      <c r="T1" t="str">
-        <f>IF(ISBLANK(recommendations!V1),"",recommendations!V1)</f>
-        <v>Thiamin</v>
-      </c>
-      <c r="U1" t="str">
-        <f>IF(ISBLANK(recommendations!W1),"",recommendations!W1)</f>
-        <v>Riboflavin</v>
-      </c>
-      <c r="V1" t="str">
-        <f>IF(ISBLANK(recommendations!X1),"",recommendations!X1)</f>
-        <v>Niacin</v>
-      </c>
-      <c r="W1" t="str">
-        <f>IF(ISBLANK(recommendations!Y1),"",recommendations!Y1)</f>
-        <v>Vitamin B6</v>
-      </c>
-      <c r="X1" t="str">
-        <f>IF(ISBLANK(recommendations!Z1),"",recommendations!Z1)</f>
-        <v>Folat</v>
-      </c>
-      <c r="Y1" t="str">
-        <f>IF(ISBLANK(recommendations!AA1),"",recommendations!AA1)</f>
-        <v>Pantothensäure</v>
-      </c>
-      <c r="Z1" t="str">
-        <f>IF(ISBLANK(recommendations!AB1),"",recommendations!AB1)</f>
-        <v>Biotin</v>
-      </c>
-      <c r="AA1" t="str">
-        <f>IF(ISBLANK(recommendations!AC1),"",recommendations!AC1)</f>
-        <v>Vitamin B12 (Cobalamine)</v>
-      </c>
-      <c r="AB1" t="str">
-        <f>IF(ISBLANK(recommendations!AD1),"",recommendations!AD1)</f>
-        <v>Vitamin C</v>
-      </c>
-      <c r="AC1" t="str">
-        <f>IF(ISBLANK(recommendations!AE1),"",recommendations!AE1)</f>
-        <v>Natrium</v>
-      </c>
-      <c r="AD1" t="str">
-        <f>IF(ISBLANK(recommendations!AF1),"",recommendations!AF1)</f>
-        <v>Chlorid</v>
-      </c>
-      <c r="AE1" t="str">
-        <f>IF(ISBLANK(recommendations!AG1),"",recommendations!AG1)</f>
-        <v>Kalium</v>
-      </c>
-      <c r="AF1" t="str">
-        <f>IF(ISBLANK(recommendations!AH1),"",recommendations!AH1)</f>
-        <v>Calcium</v>
-      </c>
-      <c r="AG1" t="str">
-        <f>IF(ISBLANK(recommendations!AI1),"",recommendations!AI1)</f>
-        <v>Phosphor</v>
-      </c>
-      <c r="AH1" t="str">
-        <f>IF(ISBLANK(recommendations!AJ1),"",recommendations!AJ1)</f>
-        <v>Magnesium</v>
-      </c>
-      <c r="AI1" t="str">
-        <f>IF(ISBLANK(recommendations!AK1),"",recommendations!AK1)</f>
-        <v>Eisen</v>
-      </c>
-      <c r="AJ1" t="str">
-        <f>IF(ISBLANK(recommendations!AL1),"",recommendations!AL1)</f>
-        <v>Jod</v>
-      </c>
-      <c r="AK1" t="str">
-        <f>IF(ISBLANK(recommendations!AM1),"",recommendations!AM1)</f>
-        <v>Fluorid</v>
-      </c>
-      <c r="AL1" t="str">
-        <f>IF(ISBLANK(recommendations!AN1),"",recommendations!AN1)</f>
-        <v>Zink</v>
-      </c>
-      <c r="AM1" t="str">
-        <f>IF(ISBLANK(recommendations!AQ1),"",recommendations!AQ1)</f>
-        <v>Selen</v>
-      </c>
-      <c r="AN1" t="str">
-        <f>IF(ISBLANK(recommendations!AR1),"",recommendations!AR1)</f>
-        <v>Kupfer</v>
-      </c>
-      <c r="AO1" t="str">
-        <f>IF(ISBLANK(recommendations!AS1),"",recommendations!AS1)</f>
-        <v>Mangan</v>
-      </c>
-      <c r="AP1" t="str">
-        <f>IF(ISBLANK(recommendations!AT1),"",recommendations!AT1)</f>
-        <v>Chrom</v>
-      </c>
-      <c r="AQ1" t="str">
-        <f>IF(ISBLANK(recommendations!AU1),"",recommendations!AU1)</f>
-        <v>Molybdän</v>
-      </c>
-      <c r="AR1" t="str">
-        <f>IF(ISBLANK(recommendations!AV1),"",recommendations!AV1)</f>
-        <v>Wasser</v>
-      </c>
-    </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A2" t="str">
-        <f>IF(ISBLANK(recommendations!A2),"",recommendations!A2)</f>
-        <v>Einheit</v>
-      </c>
-      <c r="B2" t="str">
-        <f>IF(ISBLANK(recommendations!B2),"",recommendations!B2)</f>
-        <v/>
-      </c>
-      <c r="C2" t="str">
-        <f>IF(ISBLANK(recommendations!C2),"",recommendations!C2)</f>
-        <v/>
-      </c>
-      <c r="D2" t="str">
-        <f>IF(ISBLANK(recommendations!D2),"",recommendations!D2)</f>
-        <v>kcal/Tag</v>
-      </c>
-      <c r="E2" t="str">
-        <f>IF(ISBLANK(recommendations!G2),"",recommendations!G2)</f>
-        <v>% der Energie</v>
-      </c>
-      <c r="F2" t="str">
-        <f>IF(ISBLANK(recommendations!H2),"",recommendations!H2)</f>
-        <v>g/kg KG/Tag</v>
-      </c>
-      <c r="G2" t="str">
-        <f>IF(ISBLANK(recommendations!I2),"",recommendations!I2)</f>
-        <v>% der Energie</v>
-      </c>
-      <c r="H2" t="str">
-        <f>IF(ISBLANK(recommendations!J2),"",recommendations!J2)</f>
-        <v>% der Energie</v>
-      </c>
-      <c r="I2" t="str">
-        <f>IF(ISBLANK(recommendations!K2),"",recommendations!K2)</f>
-        <v>% der Energie</v>
-      </c>
-      <c r="J2" t="str">
-        <f>IF(ISBLANK(recommendations!L2),"",recommendations!L2)</f>
-        <v>% der Energie</v>
-      </c>
-      <c r="K2" t="str">
-        <f>IF(ISBLANK(recommendations!M2),"",recommendations!M2)</f>
-        <v>% der Energie</v>
-      </c>
-      <c r="L2" t="str">
-        <f>IF(ISBLANK(recommendations!N2),"",recommendations!N2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="M2" t="str">
-        <f>IF(ISBLANK(recommendations!O2),"",recommendations!O2)</f>
-        <v>% der Energie</v>
-      </c>
-      <c r="N2" t="str">
-        <f>IF(ISBLANK(recommendations!P2),"",recommendations!P2)</f>
-        <v>g/Tag</v>
-      </c>
-      <c r="O2" t="str">
-        <f>IF(ISBLANK(recommendations!Q2),"",recommendations!Q2)</f>
-        <v>g/Tag</v>
-      </c>
-      <c r="P2" t="str">
-        <f>IF(ISBLANK(recommendations!R2),"",recommendations!R2)</f>
-        <v>µg-RAE/Tag</v>
-      </c>
-      <c r="Q2" t="str">
-        <f>IF(ISBLANK(recommendations!S2),"",recommendations!S2)</f>
-        <v>µg/Tag</v>
-      </c>
-      <c r="R2" t="str">
-        <f>IF(ISBLANK(recommendations!T2),"",recommendations!T2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="S2" t="str">
-        <f>IF(ISBLANK(recommendations!U2),"",recommendations!U2)</f>
-        <v>µg/Tag</v>
-      </c>
-      <c r="T2" t="str">
-        <f>IF(ISBLANK(recommendations!V2),"",recommendations!V2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="U2" t="str">
-        <f>IF(ISBLANK(recommendations!W2),"",recommendations!W2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="V2" t="str">
-        <f>IF(ISBLANK(recommendations!X2),"",recommendations!X2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="W2" t="str">
-        <f>IF(ISBLANK(recommendations!Y2),"",recommendations!Y2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="X2" t="str">
-        <f>IF(ISBLANK(recommendations!Z2),"",recommendations!Z2)</f>
-        <v>µg/Tag</v>
-      </c>
-      <c r="Y2" t="str">
-        <f>IF(ISBLANK(recommendations!AA2),"",recommendations!AA2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="Z2" t="str">
-        <f>IF(ISBLANK(recommendations!AB2),"",recommendations!AB2)</f>
-        <v>µg/Tag</v>
-      </c>
-      <c r="AA2" t="str">
-        <f>IF(ISBLANK(recommendations!AC2),"",recommendations!AC2)</f>
-        <v>µg/Tag</v>
-      </c>
-      <c r="AB2" t="str">
-        <f>IF(ISBLANK(recommendations!AD2),"",recommendations!AD2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="AC2" t="str">
-        <f>IF(ISBLANK(recommendations!AE2),"",recommendations!AE2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="AD2" t="str">
-        <f>IF(ISBLANK(recommendations!AF2),"",recommendations!AF2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="AE2" t="str">
-        <f>IF(ISBLANK(recommendations!AG2),"",recommendations!AG2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="AF2" t="str">
-        <f>IF(ISBLANK(recommendations!AH2),"",recommendations!AH2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="AG2" t="str">
-        <f>IF(ISBLANK(recommendations!AI2),"",recommendations!AI2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="AH2" t="str">
-        <f>IF(ISBLANK(recommendations!AJ2),"",recommendations!AJ2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="AI2" t="str">
-        <f>IF(ISBLANK(recommendations!AK2),"",recommendations!AK2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="AJ2" t="str">
-        <f>IF(ISBLANK(recommendations!AL2),"",recommendations!AL2)</f>
-        <v>µg/Tag</v>
-      </c>
-      <c r="AK2" t="str">
-        <f>IF(ISBLANK(recommendations!AM2),"",recommendations!AM2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="AL2" t="str">
-        <f>IF(ISBLANK(recommendations!AN2),"",recommendations!AN2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="AM2" t="str">
-        <f>IF(ISBLANK(recommendations!AQ2),"",recommendations!AQ2)</f>
-        <v>µg/Tag</v>
-      </c>
-      <c r="AN2" t="str">
-        <f>IF(ISBLANK(recommendations!AR2),"",recommendations!AR2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="AO2" t="str">
-        <f>IF(ISBLANK(recommendations!AS2),"",recommendations!AS2)</f>
-        <v>mg/Tag</v>
-      </c>
-      <c r="AP2" t="str">
-        <f>IF(ISBLANK(recommendations!AT2),"",recommendations!AT2)</f>
-        <v>µg/Tag</v>
-      </c>
-      <c r="AQ2" t="str">
-        <f>IF(ISBLANK(recommendations!AU2),"",recommendations!AU2)</f>
-        <v>µg/Tag</v>
-      </c>
-      <c r="AR2" t="str">
-        <f>IF(ISBLANK(recommendations!AV2),"",recommendations!AV2)</f>
-        <v>ml/Tag</v>
-      </c>
-    </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f>IF(ISBLANK(recommendations!A3),"",recommendations!A3)</f>
-        <v>Bemerkung</v>
-      </c>
-      <c r="B3" t="str">
-        <f>IF(ISBLANK(recommendations!B3),"",recommendations!B3)</f>
-        <v/>
-      </c>
-      <c r="C3" t="str">
-        <f>IF(ISBLANK(recommendations!C3),"",recommendations!C3)</f>
-        <v/>
-      </c>
-      <c r="E3" t="str">
-        <f>IF(ISBLANK(recommendations!G3),"",recommendations!G3)</f>
-        <v/>
-      </c>
-      <c r="F3" t="str">
-        <f>IF(ISBLANK(recommendations!H3),"",recommendations!H3)</f>
-        <v/>
-      </c>
-      <c r="G3" t="s">
-        <v>191</v>
-      </c>
-      <c r="H3" t="s">
-        <v>192</v>
-      </c>
-      <c r="I3" t="s">
-        <v>193</v>
-      </c>
-      <c r="J3" t="str">
-        <f>IF(ISBLANK(recommendations!L3),"",recommendations!L3)</f>
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <f>IF(ISBLANK(recommendations!M3),"",recommendations!M3)</f>
-        <v/>
-      </c>
-      <c r="L3" t="str">
-        <f>IF(ISBLANK(recommendations!N3),"",recommendations!N3)</f>
-        <v/>
-      </c>
-      <c r="M3" t="s">
-        <v>192</v>
-      </c>
-      <c r="N3" t="s">
-        <v>192</v>
-      </c>
-      <c r="O3" t="str">
-        <f>IF(ISBLANK(recommendations!Q3),"",recommendations!Q3)</f>
-        <v>tolerierbare Gesamtzufuhrmenge</v>
-      </c>
-      <c r="P3" t="str">
-        <f>IF(ISBLANK(recommendations!R3),"",recommendations!R3)</f>
-        <v/>
-      </c>
-      <c r="Q3" t="str">
-        <f>IF(ISBLANK(recommendations!S3),"",recommendations!S3)</f>
-        <v>bei fehlender endogener Synthese</v>
-      </c>
-      <c r="R3" t="str">
-        <f>IF(ISBLANK(recommendations!T3),"",recommendations!T3)</f>
-        <v/>
-      </c>
-      <c r="S3" t="str">
-        <f>IF(ISBLANK(recommendations!U3),"",recommendations!U3)</f>
-        <v/>
-      </c>
-      <c r="T3" t="str">
-        <f>IF(ISBLANK(recommendations!V3),"",recommendations!V3)</f>
-        <v/>
-      </c>
-      <c r="U3" t="str">
-        <f>IF(ISBLANK(recommendations!W3),"",recommendations!W3)</f>
-        <v/>
-      </c>
-      <c r="V3" t="str">
-        <f>IF(ISBLANK(recommendations!X3),"",recommendations!X3)</f>
-        <v/>
-      </c>
-      <c r="W3" t="str">
-        <f>IF(ISBLANK(recommendations!Y3),"",recommendations!Y3)</f>
-        <v/>
-      </c>
-      <c r="X3" t="str">
-        <f>IF(ISBLANK(recommendations!Z3),"",recommendations!Z3)</f>
-        <v>Supplementationshinweis beachten</v>
-      </c>
-      <c r="Y3" t="str">
-        <f>IF(ISBLANK(recommendations!AA3),"",recommendations!AA3)</f>
-        <v/>
-      </c>
-      <c r="Z3" t="str">
-        <f>IF(ISBLANK(recommendations!AB3),"",recommendations!AB3)</f>
-        <v/>
-      </c>
-      <c r="AA3" t="str">
-        <f>IF(ISBLANK(recommendations!AC3),"",recommendations!AC3)</f>
-        <v/>
-      </c>
-      <c r="AB3" t="str">
-        <f>IF(ISBLANK(recommendations!AD3),"",recommendations!AD3)</f>
-        <v/>
-      </c>
-      <c r="AC3" t="str">
-        <f>IF(ISBLANK(recommendations!AE3),"",recommendations!AE3)</f>
-        <v/>
-      </c>
-      <c r="AD3" t="str">
-        <f>IF(ISBLANK(recommendations!AF3),"",recommendations!AF3)</f>
-        <v/>
-      </c>
-      <c r="AE3" t="str">
-        <f>IF(ISBLANK(recommendations!AG3),"",recommendations!AG3)</f>
-        <v/>
-      </c>
-      <c r="AF3" t="str">
-        <f>IF(ISBLANK(recommendations!AH3),"",recommendations!AH3)</f>
-        <v/>
-      </c>
-      <c r="AG3" t="str">
-        <f>IF(ISBLANK(recommendations!AI3),"",recommendations!AI3)</f>
-        <v/>
-      </c>
-      <c r="AH3" t="str">
-        <f>IF(ISBLANK(recommendations!AJ3),"",recommendations!AJ3)</f>
-        <v/>
-      </c>
-      <c r="AI3" t="str">
-        <f>IF(ISBLANK(recommendations!AK3),"",recommendations!AK3)</f>
-        <v/>
-      </c>
-      <c r="AJ3" t="str">
-        <f>IF(ISBLANK(recommendations!AL3),"",recommendations!AL3)</f>
-        <v/>
-      </c>
-      <c r="AK3" t="str">
-        <f>IF(ISBLANK(recommendations!AM3),"",recommendations!AM3)</f>
-        <v/>
-      </c>
-      <c r="AL3" t="s">
-        <v>193</v>
-      </c>
-      <c r="AM3" t="str">
-        <f>IF(ISBLANK(recommendations!AQ3),"",recommendations!AQ3)</f>
-        <v/>
-      </c>
-      <c r="AN3" t="s">
-        <v>194</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>194</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>194</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>194</v>
-      </c>
-      <c r="AR3" t="str">
-        <f>IF(ISBLANK(recommendations!AV3),"",recommendations!AV3)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <f>IF(ISBLANK(recommendations!A4),"",recommendations!A4)</f>
-        <v>Kategorie</v>
-      </c>
-      <c r="B4" t="str">
-        <f>IF(ISBLANK(recommendations!B4),"",recommendations!B4)</f>
-        <v/>
-      </c>
-      <c r="C4" t="str">
-        <f>IF(ISBLANK(recommendations!C4),"",recommendations!C4)</f>
-        <v/>
-      </c>
-      <c r="D4" t="str">
-        <f>IF(ISBLANK(recommendations!D4),"",recommendations!D4)</f>
-        <v>Richtwert</v>
-      </c>
-      <c r="E4" t="str">
-        <f>IF(ISBLANK(recommendations!G4),"",recommendations!G4)</f>
-        <v>Richtwert</v>
-      </c>
-      <c r="F4" t="str">
-        <f>IF(ISBLANK(recommendations!H4),"",recommendations!H4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="H4" t="str">
-        <f>IF(ISBLANK(recommendations!J4),"",recommendations!J4)</f>
-        <v>-</v>
-      </c>
-      <c r="I4" t="str">
-        <f>IF(ISBLANK(recommendations!K4),"",recommendations!K4)</f>
-        <v>-</v>
-      </c>
-      <c r="J4" t="str">
-        <f>IF(ISBLANK(recommendations!L4),"",recommendations!L4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="K4" t="str">
-        <f>IF(ISBLANK(recommendations!M4),"",recommendations!M4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="L4" t="str">
-        <f>IF(ISBLANK(recommendations!N4),"",recommendations!N4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="M4" t="str">
-        <f>IF(ISBLANK(recommendations!O4),"",recommendations!O4)</f>
-        <v>Richtwert</v>
-      </c>
-      <c r="N4" t="str">
-        <f>IF(ISBLANK(recommendations!P4),"",recommendations!P4)</f>
-        <v>Richtwert</v>
-      </c>
-      <c r="O4" t="str">
-        <f>IF(ISBLANK(recommendations!Q4),"",recommendations!Q4)</f>
-        <v>Richtwert</v>
-      </c>
-      <c r="P4" t="str">
-        <f>IF(ISBLANK(recommendations!R4),"",recommendations!R4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="Q4" t="str">
-        <f>IF(ISBLANK(recommendations!S4),"",recommendations!S4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="R4" t="str">
-        <f>IF(ISBLANK(recommendations!T4),"",recommendations!T4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="S4" t="str">
-        <f>IF(ISBLANK(recommendations!U4),"",recommendations!U4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="T4" t="str">
-        <f>IF(ISBLANK(recommendations!V4),"",recommendations!V4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="U4" t="str">
-        <f>IF(ISBLANK(recommendations!W4),"",recommendations!W4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="V4" t="str">
-        <f>IF(ISBLANK(recommendations!X4),"",recommendations!X4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="W4" t="str">
-        <f>IF(ISBLANK(recommendations!Y4),"",recommendations!Y4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="X4" t="str">
-        <f>IF(ISBLANK(recommendations!Z4),"",recommendations!Z4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="Y4" t="str">
-        <f>IF(ISBLANK(recommendations!AA4),"",recommendations!AA4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="Z4" t="str">
-        <f>IF(ISBLANK(recommendations!AB4),"",recommendations!AB4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="AA4" t="str">
-        <f>IF(ISBLANK(recommendations!AC4),"",recommendations!AC4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="AB4" t="str">
-        <f>IF(ISBLANK(recommendations!AD4),"",recommendations!AD4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="AC4" t="str">
-        <f>IF(ISBLANK(recommendations!AE4),"",recommendations!AE4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="AD4" t="str">
-        <f>IF(ISBLANK(recommendations!AF4),"",recommendations!AF4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="AE4" t="str">
-        <f>IF(ISBLANK(recommendations!AG4),"",recommendations!AG4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="AF4" t="str">
-        <f>IF(ISBLANK(recommendations!AH4),"",recommendations!AH4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="AG4" t="str">
-        <f>IF(ISBLANK(recommendations!AI4),"",recommendations!AI4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="AH4" t="str">
-        <f>IF(ISBLANK(recommendations!AJ4),"",recommendations!AJ4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="AI4" t="str">
-        <f>IF(ISBLANK(recommendations!AK4),"",recommendations!AK4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="AJ4" t="str">
-        <f>IF(ISBLANK(recommendations!AL4),"",recommendations!AL4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="AK4" t="str">
-        <f>IF(ISBLANK(recommendations!AM4),"",recommendations!AM4)</f>
-        <v>Richtwert</v>
-      </c>
-      <c r="AL4" t="str">
-        <f>IF(ISBLANK(recommendations!AN4),"",recommendations!AN4)</f>
-        <v>Empfohlene Zufuhr</v>
-      </c>
-      <c r="AM4" t="str">
-        <f>IF(ISBLANK(recommendations!AQ4),"",recommendations!AQ4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="AN4" t="str">
-        <f>IF(ISBLANK(recommendations!AR4),"",recommendations!AR4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="AO4" t="str">
-        <f>IF(ISBLANK(recommendations!AS4),"",recommendations!AS4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="AP4" t="str">
-        <f>IF(ISBLANK(recommendations!AT4),"",recommendations!AT4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="AQ4" t="str">
-        <f>IF(ISBLANK(recommendations!AU4),"",recommendations!AU4)</f>
-        <v>Schätzwert</v>
-      </c>
-      <c r="AR4" t="str">
-        <f>IF(ISBLANK(recommendations!AV4),"",recommendations!AV4)</f>
-        <v>Richtwert</v>
-      </c>
-    </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f>IF(ISBLANK(recommendations!A5),"",recommendations!A5)</f>
-        <v>Fussnoten</v>
-      </c>
-      <c r="B5" t="str">
-        <f>IF(ISBLANK(recommendations!B5),"",recommendations!B5)</f>
-        <v/>
-      </c>
-      <c r="C5" t="str">
-        <f>IF(ISBLANK(recommendations!C5),"",recommendations!C5)</f>
-        <v/>
-      </c>
-      <c r="D5" t="str">
-        <f>IF(ISBLANK(recommendations!D5),"",recommendations!D5)</f>
-        <v/>
-      </c>
-      <c r="E5" t="str">
-        <f>IF(ISBLANK(recommendations!G5),"",recommendations!G5)</f>
-        <v>ag,aj,c,af</v>
-      </c>
-      <c r="F5" t="str">
-        <f>IF(ISBLANK(recommendations!H5),"",recommendations!H5)</f>
-        <v>a</v>
-      </c>
-      <c r="G5" t="str">
-        <f>IF(ISBLANK(recommendations!I5),"",recommendations!I5)</f>
-        <v/>
-      </c>
-      <c r="H5" t="str">
-        <f>IF(ISBLANK(recommendations!J5),"",recommendations!J5)</f>
-        <v/>
-      </c>
-      <c r="I5" t="str">
-        <f>IF(ISBLANK(recommendations!K5),"",recommendations!K5)</f>
-        <v/>
-      </c>
-      <c r="J5" t="str">
-        <f>IF(ISBLANK(recommendations!L5),"",recommendations!L5)</f>
-        <v/>
-      </c>
-      <c r="K5" t="str">
-        <f>IF(ISBLANK(recommendations!M5),"",recommendations!M5)</f>
-        <v/>
-      </c>
-      <c r="L5" t="str">
-        <f>IF(ISBLANK(recommendations!N5),"",recommendations!N5)</f>
-        <v/>
-      </c>
-      <c r="M5" t="str">
-        <f>IF(ISBLANK(recommendations!O5),"",recommendations!O5)</f>
-        <v>ai,aj</v>
-      </c>
-      <c r="N5" t="str">
-        <f>IF(ISBLANK(recommendations!P5),"",recommendations!P5)</f>
-        <v>ap</v>
-      </c>
-      <c r="O5" t="str">
-        <f>IF(ISBLANK(recommendations!Q5),"",recommendations!Q5)</f>
-        <v>ak</v>
-      </c>
-      <c r="P5" t="str">
-        <f>IF(ISBLANK(recommendations!R5),"",recommendations!R5)</f>
-        <v>d</v>
-      </c>
-      <c r="Q5" t="str">
-        <f>IF(ISBLANK(recommendations!S5),"",recommendations!S5)</f>
-        <v>e,al</v>
-      </c>
-      <c r="R5" t="str">
-        <f>IF(ISBLANK(recommendations!T5),"",recommendations!T5)</f>
-        <v>g</v>
-      </c>
-      <c r="S5" t="str">
-        <f>IF(ISBLANK(recommendations!U5),"",recommendations!U5)</f>
-        <v/>
-      </c>
-      <c r="T5" t="str">
-        <f>IF(ISBLANK(recommendations!V5),"",recommendations!V5)</f>
-        <v>j</v>
-      </c>
-      <c r="U5" t="str">
-        <f>IF(ISBLANK(recommendations!W5),"",recommendations!W5)</f>
-        <v>j</v>
-      </c>
-      <c r="V5" t="str">
-        <f>IF(ISBLANK(recommendations!X5),"",recommendations!X5)</f>
-        <v>i,j</v>
-      </c>
-      <c r="W5" t="str">
-        <f>IF(ISBLANK(recommendations!Y5),"",recommendations!Y5)</f>
-        <v/>
-      </c>
-      <c r="X5" t="str">
-        <f>IF(ISBLANK(recommendations!Z5),"",recommendations!Z5)</f>
-        <v>m,n</v>
-      </c>
-      <c r="Y5" t="str">
-        <f>IF(ISBLANK(recommendations!AA5),"",recommendations!AA5)</f>
-        <v/>
-      </c>
-      <c r="Z5" t="str">
-        <f>IF(ISBLANK(recommendations!AB5),"",recommendations!AB5)</f>
-        <v/>
-      </c>
-      <c r="AA5" t="str">
-        <f>IF(ISBLANK(recommendations!AC5),"",recommendations!AC5)</f>
-        <v/>
-      </c>
-      <c r="AB5" t="str">
-        <f>IF(ISBLANK(recommendations!AD5),"",recommendations!AD5)</f>
-        <v>p</v>
-      </c>
-      <c r="AC5" t="str">
-        <f>IF(ISBLANK(recommendations!AE5),"",recommendations!AE5)</f>
-        <v/>
-      </c>
-      <c r="AD5" t="str">
-        <f>IF(ISBLANK(recommendations!AF5),"",recommendations!AF5)</f>
-        <v/>
-      </c>
-      <c r="AE5" t="str">
-        <f>IF(ISBLANK(recommendations!AG5),"",recommendations!AG5)</f>
-        <v/>
-      </c>
-      <c r="AF5" t="str">
-        <f>IF(ISBLANK(recommendations!AH5),"",recommendations!AH5)</f>
-        <v/>
-      </c>
-      <c r="AG5" t="str">
-        <f>IF(ISBLANK(recommendations!AI5),"",recommendations!AI5)</f>
-        <v/>
-      </c>
-      <c r="AH5" t="str">
-        <f>IF(ISBLANK(recommendations!AJ5),"",recommendations!AJ5)</f>
-        <v/>
-      </c>
-      <c r="AI5" t="str">
-        <f>IF(ISBLANK(recommendations!AK5),"",recommendations!AK5)</f>
-        <v>v</v>
-      </c>
-      <c r="AJ5" t="str">
-        <f>IF(ISBLANK(recommendations!AL5),"",recommendations!AL5)</f>
-        <v/>
-      </c>
-      <c r="AK5" t="str">
-        <f>IF(ISBLANK(recommendations!AM5),"",recommendations!AM5)</f>
-        <v>am,an</v>
-      </c>
-      <c r="AL5" t="str">
-        <f>IF(ISBLANK(recommendations!AN5),"",recommendations!AN5)</f>
-        <v>x,y1</v>
-      </c>
-      <c r="AM5" t="str">
-        <f>IF(ISBLANK(recommendations!AQ5),"",recommendations!AQ5)</f>
-        <v/>
-      </c>
-      <c r="AN5" t="str">
-        <f>IF(ISBLANK(recommendations!AR5),"",recommendations!AR5)</f>
-        <v/>
-      </c>
-      <c r="AO5" t="str">
-        <f>IF(ISBLANK(recommendations!AS5),"",recommendations!AS5)</f>
-        <v/>
-      </c>
-      <c r="AP5" t="str">
-        <f>IF(ISBLANK(recommendations!AT5),"",recommendations!AT5)</f>
-        <v/>
-      </c>
-      <c r="AQ5" t="str">
-        <f>IF(ISBLANK(recommendations!AU5),"",recommendations!AU5)</f>
-        <v/>
-      </c>
-      <c r="AR5" t="str">
-        <f>IF(ISBLANK(recommendations!AV5),"",recommendations!AV5)</f>
-        <v>s</v>
-      </c>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6" t="str">
-        <f>IF(ISBLANK(recommendations!B6),"",recommendations!B6)</f>
-        <v>Ewachsene 25 bis unter 51 Jahre (Weiblich)</v>
-      </c>
-      <c r="C6" t="str">
-        <f>IF(ISBLANK(recommendations!C6),"",recommendations!C6)</f>
-        <v>Weiblich</v>
-      </c>
-      <c r="D6" s="2">
-        <f>(recommendations!D6+recommendations!E6+recommendations!F6)/3</f>
-        <v>2100</v>
-      </c>
-      <c r="E6" t="str">
-        <f>IF(ISBLANK(recommendations!G6),"",recommendations!G6)</f>
-        <v>30</v>
-      </c>
-      <c r="F6" t="str">
-        <f>IF(ISBLANK(recommendations!H6),"",recommendations!H6)</f>
-        <v>0,8</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>10</v>
-      </c>
-      <c r="I6">
-        <v>8.5</v>
-      </c>
-      <c r="J6" t="str">
-        <f>IF(ISBLANK(recommendations!L6),"",recommendations!L6)</f>
-        <v>2,5</v>
-      </c>
-      <c r="K6" t="str">
-        <f>IF(ISBLANK(recommendations!M6),"",recommendations!M6)</f>
-        <v>0,5</v>
-      </c>
-      <c r="L6" t="str">
-        <f>IF(ISBLANK(recommendations!N6),"",recommendations!N6)</f>
-        <v>250</v>
-      </c>
-      <c r="M6">
-        <v>50</v>
-      </c>
-      <c r="N6">
-        <v>30</v>
-      </c>
-      <c r="O6" t="str">
-        <f>IF(ISBLANK(recommendations!Q6),"",recommendations!Q6)</f>
-        <v>10</v>
-      </c>
-      <c r="P6" t="str">
-        <f>IF(ISBLANK(recommendations!R6),"",recommendations!R6)</f>
-        <v>700</v>
-      </c>
-      <c r="Q6" t="str">
-        <f>IF(ISBLANK(recommendations!S6),"",recommendations!S6)</f>
-        <v>20</v>
-      </c>
-      <c r="R6" t="str">
-        <f>IF(ISBLANK(recommendations!T6),"",recommendations!T6)</f>
-        <v>12</v>
-      </c>
-      <c r="S6" t="str">
-        <f>IF(ISBLANK(recommendations!U6),"",recommendations!U6)</f>
-        <v>60</v>
-      </c>
-      <c r="T6" t="str">
-        <f>IF(ISBLANK(recommendations!V6),"",recommendations!V6)</f>
-        <v>1,0</v>
-      </c>
-      <c r="U6" t="str">
-        <f>IF(ISBLANK(recommendations!W6),"",recommendations!W6)</f>
-        <v>1,1</v>
-      </c>
-      <c r="V6" t="str">
-        <f>IF(ISBLANK(recommendations!X6),"",recommendations!X6)</f>
-        <v>12</v>
-      </c>
-      <c r="W6" t="str">
-        <f>IF(ISBLANK(recommendations!Y6),"",recommendations!Y6)</f>
-        <v>1,4</v>
-      </c>
-      <c r="X6" t="str">
-        <f>IF(ISBLANK(recommendations!Z6),"",recommendations!Z6)</f>
-        <v>300</v>
-      </c>
-      <c r="Y6" t="str">
-        <f>IF(ISBLANK(recommendations!AA6),"",recommendations!AA6)</f>
-        <v>5</v>
-      </c>
-      <c r="Z6" t="str">
-        <f>IF(ISBLANK(recommendations!AB6),"",recommendations!AB6)</f>
-        <v>40</v>
-      </c>
-      <c r="AA6" t="str">
-        <f>IF(ISBLANK(recommendations!AC6),"",recommendations!AC6)</f>
-        <v>4,0</v>
-      </c>
-      <c r="AB6" t="str">
-        <f>IF(ISBLANK(recommendations!AD6),"",recommendations!AD6)</f>
-        <v>95</v>
-      </c>
-      <c r="AC6" t="str">
-        <f>IF(ISBLANK(recommendations!AE6),"",recommendations!AE6)</f>
-        <v>1500</v>
-      </c>
-      <c r="AD6" t="str">
-        <f>IF(ISBLANK(recommendations!AF6),"",recommendations!AF6)</f>
-        <v>2300</v>
-      </c>
-      <c r="AE6" t="str">
-        <f>IF(ISBLANK(recommendations!AG6),"",recommendations!AG6)</f>
-        <v>4000</v>
-      </c>
-      <c r="AF6" t="str">
-        <f>IF(ISBLANK(recommendations!AH6),"",recommendations!AH6)</f>
-        <v>1000</v>
-      </c>
-      <c r="AG6" t="str">
-        <f>IF(ISBLANK(recommendations!AI6),"",recommendations!AI6)</f>
-        <v>700</v>
-      </c>
-      <c r="AH6" t="str">
-        <f>IF(ISBLANK(recommendations!AJ6),"",recommendations!AJ6)</f>
-        <v>300</v>
-      </c>
-      <c r="AI6" t="str">
-        <f>IF(ISBLANK(recommendations!AK6),"",recommendations!AK6)</f>
-        <v>15</v>
-      </c>
-      <c r="AJ6" t="str">
-        <f>IF(ISBLANK(recommendations!AL6),"",recommendations!AL6)</f>
-        <v>200</v>
-      </c>
-      <c r="AK6" t="str">
-        <f>IF(ISBLANK(recommendations!AM6),"",recommendations!AM6)</f>
-        <v>3,1</v>
-      </c>
-      <c r="AL6">
-        <f>(recommendations!AN6+recommendations!AO6+recommendations!AP6)/3</f>
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="AM6" t="str">
-        <f>IF(ISBLANK(recommendations!AQ6),"",recommendations!AQ6)</f>
-        <v>60</v>
-      </c>
-      <c r="AN6">
-        <v>1.25</v>
-      </c>
-      <c r="AO6">
-        <v>3.5</v>
-      </c>
-      <c r="AP6">
-        <v>65</v>
-      </c>
-      <c r="AQ6">
-        <v>75</v>
-      </c>
-      <c r="AR6" t="str">
-        <f>IF(ISBLANK(recommendations!AV6),"",recommendations!AV6)</f>
-        <v>1410</v>
-      </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="str">
-        <f>IF(ISBLANK(recommendations!B7),"",recommendations!B7)</f>
-        <v>Ewachsene 25 bis unter 51 Jahre (Männlich)</v>
-      </c>
-      <c r="C7" t="str">
-        <f>IF(ISBLANK(recommendations!C7),"",recommendations!C7)</f>
-        <v>Männlich</v>
-      </c>
-      <c r="D7" s="2">
-        <f>(recommendations!D7+recommendations!E7+recommendations!F7)/3</f>
-        <v>2666.6666666666665</v>
-      </c>
-      <c r="E7" t="str">
-        <f>IF(ISBLANK(recommendations!G7),"",recommendations!G7)</f>
-        <v>30</v>
-      </c>
-      <c r="F7" t="str">
-        <f>IF(ISBLANK(recommendations!H7),"",recommendations!H7)</f>
-        <v>0,8</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>10</v>
-      </c>
-      <c r="I7">
-        <v>8.5</v>
-      </c>
-      <c r="J7" t="str">
-        <f>IF(ISBLANK(recommendations!L7),"",recommendations!L7)</f>
-        <v>2,5</v>
-      </c>
-      <c r="K7" t="str">
-        <f>IF(ISBLANK(recommendations!M7),"",recommendations!M7)</f>
-        <v>0,5</v>
-      </c>
-      <c r="L7" t="str">
-        <f>IF(ISBLANK(recommendations!N7),"",recommendations!N7)</f>
-        <v>250</v>
-      </c>
-      <c r="M7">
-        <v>50</v>
-      </c>
-      <c r="N7">
-        <v>30</v>
-      </c>
-      <c r="O7" t="str">
-        <f>IF(ISBLANK(recommendations!Q7),"",recommendations!Q7)</f>
-        <v>20</v>
-      </c>
-      <c r="P7" t="str">
-        <f>IF(ISBLANK(recommendations!R7),"",recommendations!R7)</f>
-        <v>850</v>
-      </c>
-      <c r="Q7" t="str">
-        <f>IF(ISBLANK(recommendations!S7),"",recommendations!S7)</f>
-        <v>20</v>
-      </c>
-      <c r="R7" t="str">
-        <f>IF(ISBLANK(recommendations!T7),"",recommendations!T7)</f>
-        <v>14</v>
-      </c>
-      <c r="S7" t="str">
-        <f>IF(ISBLANK(recommendations!U7),"",recommendations!U7)</f>
-        <v>70</v>
-      </c>
-      <c r="T7" t="str">
-        <f>IF(ISBLANK(recommendations!V7),"",recommendations!V7)</f>
-        <v>1,2</v>
-      </c>
-      <c r="U7" t="str">
-        <f>IF(ISBLANK(recommendations!W7),"",recommendations!W7)</f>
-        <v>1,4</v>
-      </c>
-      <c r="V7" t="str">
-        <f>IF(ISBLANK(recommendations!X7),"",recommendations!X7)</f>
-        <v>15</v>
-      </c>
-      <c r="W7" t="str">
-        <f>IF(ISBLANK(recommendations!Y7),"",recommendations!Y7)</f>
-        <v>1,6</v>
-      </c>
-      <c r="X7" t="str">
-        <f>IF(ISBLANK(recommendations!Z7),"",recommendations!Z7)</f>
-        <v>300</v>
-      </c>
-      <c r="Y7" t="str">
-        <f>IF(ISBLANK(recommendations!AA7),"",recommendations!AA7)</f>
-        <v>5</v>
-      </c>
-      <c r="Z7" t="str">
-        <f>IF(ISBLANK(recommendations!AB7),"",recommendations!AB7)</f>
-        <v>40</v>
-      </c>
-      <c r="AA7" t="str">
-        <f>IF(ISBLANK(recommendations!AC7),"",recommendations!AC7)</f>
-        <v>4,0</v>
-      </c>
-      <c r="AB7" t="str">
-        <f>IF(ISBLANK(recommendations!AD7),"",recommendations!AD7)</f>
-        <v>110</v>
-      </c>
-      <c r="AC7" t="str">
-        <f>IF(ISBLANK(recommendations!AE7),"",recommendations!AE7)</f>
-        <v>1500</v>
-      </c>
-      <c r="AD7" t="str">
-        <f>IF(ISBLANK(recommendations!AF7),"",recommendations!AF7)</f>
-        <v>2300</v>
-      </c>
-      <c r="AE7" t="str">
-        <f>IF(ISBLANK(recommendations!AG7),"",recommendations!AG7)</f>
-        <v>4000</v>
-      </c>
-      <c r="AF7" t="str">
-        <f>IF(ISBLANK(recommendations!AH7),"",recommendations!AH7)</f>
-        <v>1000</v>
-      </c>
-      <c r="AG7" t="str">
-        <f>IF(ISBLANK(recommendations!AI7),"",recommendations!AI7)</f>
-        <v>700</v>
-      </c>
-      <c r="AH7" t="str">
-        <f>IF(ISBLANK(recommendations!AJ7),"",recommendations!AJ7)</f>
-        <v>350</v>
-      </c>
-      <c r="AI7" t="str">
-        <f>IF(ISBLANK(recommendations!AK7),"",recommendations!AK7)</f>
-        <v>10</v>
-      </c>
-      <c r="AJ7" t="str">
-        <f>IF(ISBLANK(recommendations!AL7),"",recommendations!AL7)</f>
-        <v>200</v>
-      </c>
-      <c r="AK7" t="str">
-        <f>IF(ISBLANK(recommendations!AM7),"",recommendations!AM7)</f>
-        <v>3,8</v>
-      </c>
-      <c r="AL7">
-        <f>(recommendations!AN7+recommendations!AO7+recommendations!AP7)/3</f>
-        <v>13.666666666666666</v>
-      </c>
-      <c r="AM7" t="str">
-        <f>IF(ISBLANK(recommendations!AQ7),"",recommendations!AQ7)</f>
-        <v>70</v>
-      </c>
-      <c r="AN7">
-        <v>1.25</v>
-      </c>
-      <c r="AO7">
-        <v>3.5</v>
-      </c>
-      <c r="AP7">
-        <v>65</v>
-      </c>
-      <c r="AQ7">
-        <v>75</v>
-      </c>
-      <c r="AR7" t="str">
-        <f>IF(ISBLANK(recommendations!AV7),"",recommendations!AV7)</f>
-        <v>1410</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
start of the data cleaning process
</commit_message>
<xml_diff>
--- a/DGE_recommendations.xlsx
+++ b/DGE_recommendations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/321e4917f5e22f1c/Desktop/IT-Projekte/Multidimensional_Nutri-Score/Code/Multidimensional-Nutri-Score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="304" documentId="8_{03962255-4955-4F35-8BDF-772533F35B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFCB295A-9D2F-4767-8764-AADC5D232094}"/>
+  <xr:revisionPtr revIDLastSave="316" documentId="8_{03962255-4955-4F35-8BDF-772533F35B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F75F2072-2F38-4A1B-8636-E1A4495885AE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="218">
   <si>
     <t>Bevölkerungsgruppe</t>
   </si>
@@ -658,54 +658,6 @@
     <t>max (avg)</t>
   </si>
   <si>
-    <t>A (Retinoläquivalent)</t>
-  </si>
-  <si>
-    <t>A (Retinol)</t>
-  </si>
-  <si>
-    <t>A (Beta-Carotin)</t>
-  </si>
-  <si>
-    <t>B1 (Thiamin)</t>
-  </si>
-  <si>
-    <t>B2 (Riboflavin)</t>
-  </si>
-  <si>
-    <t>B3 (Niacin, Nicotinsäure)</t>
-  </si>
-  <si>
-    <t>B3 (Niacinäquivalent)</t>
-  </si>
-  <si>
-    <t>B5 (Pantothensäure)</t>
-  </si>
-  <si>
-    <t>B6 (Pyridoxin)</t>
-  </si>
-  <si>
-    <t>B7 (Biotin (Vitamin H))</t>
-  </si>
-  <si>
-    <t>B9 (gesamte Folsäure)</t>
-  </si>
-  <si>
-    <t>B12 (Cobalamin)</t>
-  </si>
-  <si>
-    <t>C (Ascorbinsäure)</t>
-  </si>
-  <si>
-    <t>D (Calciferole)</t>
-  </si>
-  <si>
-    <t>E (Tocopherole)</t>
-  </si>
-  <si>
-    <t>K ()</t>
-  </si>
-  <si>
     <t>Quelle</t>
   </si>
   <si>
@@ -713,6 +665,54 @@
   </si>
   <si>
     <t>DGE</t>
+  </si>
+  <si>
+    <t>A Retinoläquivalent (µg)</t>
+  </si>
+  <si>
+    <t>A Retinol (µg)</t>
+  </si>
+  <si>
+    <t>A Beta-Carotin (µg)</t>
+  </si>
+  <si>
+    <t>B1 Thiamin (µg)</t>
+  </si>
+  <si>
+    <t>B2 Riboflavin (µg)</t>
+  </si>
+  <si>
+    <t>B3 Niacin, Nicotinsäure (µg)</t>
+  </si>
+  <si>
+    <t>B3 Niacinäquivalent (µg)</t>
+  </si>
+  <si>
+    <t>B5 Pantothensäure (µg)</t>
+  </si>
+  <si>
+    <t>B6 Pyridoxin (µg)</t>
+  </si>
+  <si>
+    <t>B7 Biotin (Vitamin H) (µg)</t>
+  </si>
+  <si>
+    <t>B9 gesamte Folsäure (µg)</t>
+  </si>
+  <si>
+    <t>B12 Cobalamin (µg)</t>
+  </si>
+  <si>
+    <t>C Ascorbinsäure (µg)</t>
+  </si>
+  <si>
+    <t>D Calciferole (µg)</t>
+  </si>
+  <si>
+    <t>E Tocopherole (µg)</t>
+  </si>
+  <si>
+    <t>K (µg)</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F32006-BDCD-4040-96C8-0A9582070BD1}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1111,310 +1111,260 @@
         <v>195</v>
       </c>
       <c r="B1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="E1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="H1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="I1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="J1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="K1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="L1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="M1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="N1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="O1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="P1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="Q1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2">
+        <v>900</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+      <c r="D2">
+        <v>2000</v>
+      </c>
+      <c r="E2">
+        <v>1100</v>
+      </c>
+      <c r="F2">
+        <v>1200</v>
+      </c>
+      <c r="G2">
+        <v>15000</v>
+      </c>
+      <c r="H2">
+        <v>17000</v>
+      </c>
+      <c r="I2">
+        <v>6000</v>
+      </c>
+      <c r="J2">
+        <v>16000</v>
+      </c>
+      <c r="K2">
+        <v>45</v>
+      </c>
+      <c r="L2">
+        <v>400</v>
+      </c>
+      <c r="M2">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" t="s">
-        <v>61</v>
-      </c>
-      <c r="L2" t="s">
-        <v>61</v>
-      </c>
-      <c r="M2" t="s">
-        <v>61</v>
-      </c>
-      <c r="N2" t="s">
-        <v>61</v>
-      </c>
-      <c r="O2" t="s">
-        <v>61</v>
-      </c>
-      <c r="P2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>61</v>
+      <c r="N2">
+        <v>100000</v>
+      </c>
+      <c r="O2">
+        <v>20</v>
+      </c>
+      <c r="P2">
+        <v>14000</v>
+      </c>
+      <c r="Q2">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B3">
-        <v>900</v>
-      </c>
-      <c r="C3">
-        <v>2000</v>
-      </c>
-      <c r="D3">
-        <v>1000</v>
-      </c>
-      <c r="E3">
-        <v>1100</v>
-      </c>
-      <c r="F3">
-        <v>1200</v>
-      </c>
-      <c r="G3">
-        <v>15000</v>
-      </c>
-      <c r="H3">
-        <v>17000</v>
-      </c>
-      <c r="I3">
-        <v>6000</v>
-      </c>
-      <c r="J3">
-        <v>16000</v>
-      </c>
-      <c r="K3">
-        <v>45</v>
-      </c>
-      <c r="L3">
-        <v>400</v>
-      </c>
-      <c r="M3">
-        <v>4</v>
-      </c>
-      <c r="N3">
-        <v>100000</v>
-      </c>
-      <c r="O3">
-        <v>20</v>
-      </c>
-      <c r="P3">
-        <v>14000</v>
-      </c>
-      <c r="Q3">
-        <v>65</v>
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G3" t="s">
+        <v>193</v>
+      </c>
+      <c r="I3" t="s">
+        <v>193</v>
+      </c>
+      <c r="N3" t="s">
+        <v>193</v>
+      </c>
+      <c r="O3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P3" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>193</v>
+        <v>197</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>193</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>193</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>193</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>193</v>
+        <v>27</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" t="s">
+        <v>40</v>
       </c>
       <c r="N4" t="s">
-        <v>193</v>
+        <v>27</v>
       </c>
       <c r="O4" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="P4" t="s">
-        <v>193</v>
+        <v>40</v>
       </c>
       <c r="Q4" t="s">
-        <v>193</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>197</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="L5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="N5" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="O5" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="P5" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>199</v>
+      </c>
+      <c r="B6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" t="s">
+        <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>200</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>201</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>201</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>200</v>
+      </c>
+      <c r="H6" t="s">
+        <v>200</v>
+      </c>
+      <c r="I6" t="s">
+        <v>200</v>
+      </c>
+      <c r="J6" t="s">
+        <v>201</v>
+      </c>
+      <c r="K6" t="s">
+        <v>200</v>
       </c>
       <c r="L6" t="s">
-        <v>81</v>
+        <v>201</v>
+      </c>
+      <c r="M6" t="s">
+        <v>201</v>
       </c>
       <c r="N6" t="s">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="O6" t="s">
-        <v>63</v>
+        <v>201</v>
       </c>
       <c r="P6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>215</v>
-      </c>
-      <c r="B7" t="s">
-        <v>216</v>
-      </c>
-      <c r="C7" t="s">
-        <v>216</v>
-      </c>
-      <c r="D7" t="s">
-        <v>216</v>
-      </c>
-      <c r="E7" t="s">
-        <v>217</v>
-      </c>
-      <c r="F7" t="s">
-        <v>217</v>
-      </c>
-      <c r="G7" t="s">
-        <v>216</v>
-      </c>
-      <c r="H7" t="s">
-        <v>216</v>
-      </c>
-      <c r="I7" t="s">
-        <v>216</v>
-      </c>
-      <c r="J7" t="s">
-        <v>217</v>
-      </c>
-      <c r="K7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L7" t="s">
-        <v>217</v>
-      </c>
-      <c r="M7" t="s">
-        <v>217</v>
-      </c>
-      <c r="N7" t="s">
-        <v>217</v>
-      </c>
-      <c r="O7" t="s">
-        <v>217</v>
-      </c>
-      <c r="P7" t="s">
-        <v>216</v>
+        <v>200</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1426,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265B2FAF-ABBA-4113-9E4F-E2409CE22460}">
   <dimension ref="A1:AP6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2363,8 +2313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="A47" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4751,7 +4701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -4977,8 +4927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F5A0FC-0C73-492D-8E0C-7F7EF8032F1F}">
   <dimension ref="A1:AV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA27" sqref="AA27"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
refactoring and calculations of vitamin proportions
</commit_message>
<xml_diff>
--- a/DGE_recommendations.xlsx
+++ b/DGE_recommendations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/321e4917f5e22f1c/Desktop/IT-Projekte/Multidimensional_Nutri-Score/Code/Multidimensional-Nutri-Score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="316" documentId="8_{03962255-4955-4F35-8BDF-772533F35B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F75F2072-2F38-4A1B-8636-E1A4495885AE}"/>
+  <xr:revisionPtr revIDLastSave="318" documentId="8_{03962255-4955-4F35-8BDF-772533F35B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70B7D8DD-6489-4844-B4EA-D099F9784F6B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1824" yWindow="696" windowWidth="11772" windowHeight="11256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="avg_vitamins" sheetId="7" r:id="rId1"/>
@@ -1104,6 +1104,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.69921875" customWidth="1"/>
+    <col min="16" max="16" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Calculation of average mineral requirement coverage by volume and calories
</commit_message>
<xml_diff>
--- a/DGE_recommendations.xlsx
+++ b/DGE_recommendations.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/321e4917f5e22f1c/Desktop/IT-Projekte/Multidimensional_Nutri-Score/Code/Multidimensional-Nutri-Score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="318" documentId="8_{03962255-4955-4F35-8BDF-772533F35B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70B7D8DD-6489-4844-B4EA-D099F9784F6B}"/>
+  <xr:revisionPtr revIDLastSave="401" documentId="8_{03962255-4955-4F35-8BDF-772533F35B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD14EEB6-14CA-4236-B4F2-B3AF83E5E860}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1824" yWindow="696" windowWidth="11772" windowHeight="11256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="avg_vitamins" sheetId="7" r:id="rId1"/>
-    <sheet name="avg_recom" sheetId="6" r:id="rId2"/>
-    <sheet name="Referenzwerte df" sheetId="1" r:id="rId3"/>
-    <sheet name="Fußnoten" sheetId="2" r:id="rId4"/>
-    <sheet name="recommendations" sheetId="3" r:id="rId5"/>
+    <sheet name="avg_minerals" sheetId="8" r:id="rId2"/>
+    <sheet name="avg_trminerals" sheetId="9" r:id="rId3"/>
+    <sheet name="avg_recom" sheetId="6" r:id="rId4"/>
+    <sheet name="Referenzwerte df" sheetId="1" r:id="rId5"/>
+    <sheet name="Fußnoten" sheetId="2" r:id="rId6"/>
+    <sheet name="recommendations" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="220">
   <si>
     <t>Bevölkerungsgruppe</t>
   </si>
@@ -713,6 +715,12 @@
   </si>
   <si>
     <t>K (µg)</t>
+  </si>
+  <si>
+    <t>Iodid</t>
+  </si>
+  <si>
+    <t>nährwertrechner.de</t>
   </si>
 </sst>
 </file>
@@ -748,10 +756,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1097,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F32006-BDCD-4040-96C8-0A9582070BD1}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1374,11 +1385,375 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD441CA-8DDA-4EAF-B747-DA2BB3763119}">
+  <dimension ref="A1:Q7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="3">
+        <v>350</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" t="s">
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
+        <v>201</v>
+      </c>
+      <c r="G7" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73AA07A8-2B1A-4150-A43D-648DDF76D631}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="3">
+        <v>12500</v>
+      </c>
+      <c r="C3" s="3">
+        <v>11000</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1250</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3500</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3800</v>
+      </c>
+      <c r="G3" s="3">
+        <v>200</v>
+      </c>
+      <c r="H3" s="3">
+        <v>65</v>
+      </c>
+      <c r="I3" s="3">
+        <v>65</v>
+      </c>
+      <c r="J3" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F5" t="s">
+        <v>193</v>
+      </c>
+      <c r="H5" t="s">
+        <v>193</v>
+      </c>
+      <c r="I5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F7" t="s">
+        <v>219</v>
+      </c>
+      <c r="G7" t="s">
+        <v>201</v>
+      </c>
+      <c r="H7" t="s">
+        <v>201</v>
+      </c>
+      <c r="I7" t="s">
+        <v>201</v>
+      </c>
+      <c r="J7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265B2FAF-ABBA-4113-9E4F-E2409CE22460}">
   <dimension ref="A1:AP6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="X1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AJ3" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2310,11 +2685,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
@@ -4698,7 +5073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
@@ -4924,7 +5299,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F5A0FC-0C73-492D-8E0C-7F7EF8032F1F}">
   <dimension ref="A1:AV10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Calculation of average trace mineral requirement coverage by volume and calories
</commit_message>
<xml_diff>
--- a/DGE_recommendations.xlsx
+++ b/DGE_recommendations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/321e4917f5e22f1c/Desktop/IT-Projekte/Multidimensional_Nutri-Score/Code/Multidimensional-Nutri-Score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="401" documentId="8_{03962255-4955-4F35-8BDF-772533F35B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD14EEB6-14CA-4236-B4F2-B3AF83E5E860}"/>
+  <xr:revisionPtr revIDLastSave="408" documentId="8_{03962255-4955-4F35-8BDF-772533F35B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D141EFCA-AC39-4159-8AD5-CD3F0AFC3FFA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="avg_vitamins" sheetId="7" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="220">
   <si>
     <t>Bevölkerungsgruppe</t>
   </si>
@@ -1106,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F32006-BDCD-4040-96C8-0A9582070BD1}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1173,209 +1173,262 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B2">
-        <v>900</v>
-      </c>
-      <c r="C2">
-        <v>1000</v>
-      </c>
-      <c r="D2">
-        <v>2000</v>
-      </c>
-      <c r="E2">
-        <v>1100</v>
-      </c>
-      <c r="F2">
-        <v>1200</v>
-      </c>
-      <c r="G2">
-        <v>15000</v>
-      </c>
-      <c r="H2">
-        <v>17000</v>
-      </c>
-      <c r="I2">
-        <v>6000</v>
-      </c>
-      <c r="J2">
-        <v>16000</v>
-      </c>
-      <c r="K2">
-        <v>45</v>
-      </c>
-      <c r="L2">
-        <v>400</v>
-      </c>
-      <c r="M2">
         <v>4</v>
       </c>
-      <c r="N2">
-        <v>100000</v>
-      </c>
-      <c r="O2">
-        <v>20</v>
-      </c>
-      <c r="P2">
-        <v>14000</v>
-      </c>
-      <c r="Q2">
-        <v>65</v>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" t="s">
+        <v>61</v>
+      </c>
+      <c r="P2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>193</v>
-      </c>
-      <c r="E3" t="s">
-        <v>193</v>
-      </c>
-      <c r="F3" t="s">
-        <v>193</v>
-      </c>
-      <c r="G3" t="s">
-        <v>193</v>
-      </c>
-      <c r="I3" t="s">
-        <v>193</v>
-      </c>
-      <c r="N3" t="s">
-        <v>193</v>
-      </c>
-      <c r="O3" t="s">
-        <v>62</v>
-      </c>
-      <c r="P3" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>193</v>
+        <v>196</v>
+      </c>
+      <c r="B3">
+        <v>900</v>
+      </c>
+      <c r="C3">
+        <v>1000</v>
+      </c>
+      <c r="D3">
+        <v>2000</v>
+      </c>
+      <c r="E3">
+        <v>1100</v>
+      </c>
+      <c r="F3">
+        <v>1200</v>
+      </c>
+      <c r="G3">
+        <v>15000</v>
+      </c>
+      <c r="H3">
+        <v>17000</v>
+      </c>
+      <c r="I3">
+        <v>6000</v>
+      </c>
+      <c r="J3">
+        <v>16000</v>
+      </c>
+      <c r="K3">
+        <v>45</v>
+      </c>
+      <c r="L3">
+        <v>400</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>100000</v>
+      </c>
+      <c r="O3">
+        <v>20</v>
+      </c>
+      <c r="P3">
+        <v>14000</v>
+      </c>
+      <c r="Q3">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>193</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>193</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>193</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>193</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" t="s">
-        <v>40</v>
+        <v>193</v>
       </c>
       <c r="N4" t="s">
-        <v>27</v>
+        <v>193</v>
       </c>
       <c r="O4" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="P4" t="s">
-        <v>40</v>
+        <v>193</v>
       </c>
       <c r="Q4" t="s">
-        <v>40</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
       </c>
       <c r="L5" t="s">
-        <v>81</v>
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>40</v>
       </c>
       <c r="N5" t="s">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="O5" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="P5" t="s">
-        <v>66</v>
+        <v>40</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" t="s">
+        <v>81</v>
+      </c>
+      <c r="N6" t="s">
+        <v>90</v>
+      </c>
+      <c r="O6" t="s">
+        <v>63</v>
+      </c>
+      <c r="P6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>199</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>200</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>200</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>200</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>201</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>201</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>200</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>200</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I7" t="s">
         <v>200</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J7" t="s">
         <v>201</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K7" t="s">
         <v>200</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L7" t="s">
         <v>201</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M7" t="s">
         <v>201</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N7" t="s">
         <v>201</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O7" t="s">
         <v>201</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P7" t="s">
         <v>200</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q7" t="s">
         <v>201</v>
       </c>
     </row>
@@ -1388,8 +1441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD441CA-8DDA-4EAF-B747-DA2BB3763119}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>